<commit_message>
Agregado y modificado contenido en 'recursos Externos'
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\compartida\HTML\Cursos\_Ironhack Java Backend Dev\Curso\Midterm_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\compartida\HTML\Cursos\_Ironhack Java Backend Dev\Curso\Midterm_Project\Proyecto_Bancario\External_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
   <si>
     <t>Request Type</t>
   </si>
@@ -46,9 +46,6 @@
     <t>/doctors</t>
   </si>
   <si>
-    <t>/patients</t>
-  </si>
-  <si>
     <t>Param Type</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>/patients/{id}</t>
   </si>
   <si>
-    <t>/patients?doctorstatus={X}</t>
-  </si>
-  <si>
     <t>/doctors/{id}?status={X}</t>
   </si>
   <si>
@@ -229,14 +223,65 @@
     <t>/accountholder</t>
   </si>
   <si>
-    <t>bienvenida del usuario X</t>
+    <t>Muestra todas sus cuentas</t>
+  </si>
+  <si>
+    <t>/accountholder/{iban}</t>
+  </si>
+  <si>
+    <t>Muestra el detalle de una especifica cuenta.</t>
+  </si>
+  <si>
+    <t>/accountholder/{iban}/withdraw</t>
+  </si>
+  <si>
+    <t>Solicitar un retiro de fondos</t>
+  </si>
+  <si>
+    <t>Realizar un deposito de fondos</t>
+  </si>
+  <si>
+    <t>/admin/accountholder/{id}/accounts</t>
+  </si>
+  <si>
+    <t>muestra las diversas cuentas de un accountholder</t>
+  </si>
+  <si>
+    <t>/admin/accountholder/{id}/accounts/{IBAN}</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Requsitos</t>
+  </si>
+  <si>
+    <t>Type, name, birthdate, address 1, address 2</t>
+  </si>
+  <si>
+    <t>Type, name, hashedKey</t>
+  </si>
+  <si>
+    <t>crear un accountholder (Opcional)</t>
+  </si>
+  <si>
+    <t>crear un ThirdParty user (Opcional)</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Modifica el saldo de la cuenta indicada</t>
+  </si>
+  <si>
+    <t>IBAN, nuevo saldo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +313,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +350,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,10 +430,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -413,23 +471,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -512,6 +572,9 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -526,26 +589,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:F17" totalsRowShown="0">
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G24" totalsRowShown="0">
+  <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="10"/>
     <tableColumn id="2" name="Request Type" dataDxfId="9"/>
     <tableColumn id="5" name="Param Type"/>
-    <tableColumn id="7" name="Usuario" dataDxfId="0"/>
+    <tableColumn id="7" name="Usuario" dataDxfId="8"/>
     <tableColumn id="3" name="Endpoint"/>
-    <tableColumn id="4" name="Response Description" dataDxfId="8"/>
+    <tableColumn id="4" name="Response Description" dataDxfId="7"/>
+    <tableColumn id="6" name="Requsitos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A12:D17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A12:D17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="4">
-    <tableColumn id="1" name="patient_id" dataDxfId="5"/>
-    <tableColumn id="2" name="name" dataDxfId="4"/>
-    <tableColumn id="3" name="date_of_birth" dataDxfId="3"/>
-    <tableColumn id="4" name="admitted_by" dataDxfId="2"/>
+    <tableColumn id="1" name="patient_id" dataDxfId="4"/>
+    <tableColumn id="2" name="name" dataDxfId="3"/>
+    <tableColumn id="3" name="date_of_birth" dataDxfId="2"/>
+    <tableColumn id="4" name="admitted_by" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -556,7 +620,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="employee_id"/>
     <tableColumn id="2" name="department"/>
-    <tableColumn id="3" name="name" dataDxfId="1"/>
+    <tableColumn id="3" name="name" dataDxfId="0"/>
     <tableColumn id="4" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -843,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,20 +919,21 @@
     <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" customWidth="1"/>
     <col min="6" max="6" width="103" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -876,10 +941,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>
@@ -887,8 +952,11 @@
       <c r="F3" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -896,196 +964,284 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>54</v>
+      <c r="D7" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>10</v>
-      </c>
-      <c r="D13" s="20"/>
+      <c r="B13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="E13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>11</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="18"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>12</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="2" t="s">
-        <v>12</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="18"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>13</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="18"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
+        <v>7</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>11</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>12</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>13</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>14</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C24">
       <formula1>"-----,PathVariable,RequestParam"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D24">
       <formula1>"Admin,AccountHolder,ThirdParty"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B24">
       <formula1>"GET,POST,PUT,PATCH,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1117,25 +1273,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="A1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1143,13 +1299,13 @@
         <v>356712</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="J3" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1161,13 +1317,13 @@
         <v>564134</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
       </c>
       <c r="J4" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1179,13 +1335,13 @@
         <v>761527</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1197,13 +1353,13 @@
         <v>166552</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J6" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1215,13 +1371,13 @@
         <v>156545</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1233,13 +1389,13 @@
         <v>172456</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J8" t="str">
         <f>CONCATENATE("INSERT INTO employees (employee_id, department, name, status) VALUES (",Tabla2[[#This Row],[employee_id]],", '",Tabla2[[#This Row],[department]],"', '",Tabla2[[#This Row],[name]],"', '",Tabla2[[#This Row],[status]],"'); ")</f>
@@ -1247,34 +1403,34 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="G12" t="s">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
       </c>
       <c r="J12" t="str">
         <f>CONCATENATE("INSERT INTO patients (patients.patient_id, patients.name, patients.date_of_birth, patients.admitted_by) VALUES (",A13,", '",B13,"', '",H13,"-",G13,"-",F13,"', ",D13,"); ")</f>
@@ -1286,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="9">
         <v>30743</v>
@@ -1316,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="9">
         <v>26310</v>
@@ -1346,7 +1502,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="9">
         <v>19886</v>
@@ -1376,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="9">
         <v>11637</v>
@@ -1406,7 +1562,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="9">
         <v>36206</v>
@@ -1463,29 +1619,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="E2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1663,36 +1819,36 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="F12" s="7"/>
       <c r="H12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1712,7 +1868,7 @@
         <v>30743</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H13">
         <f>YEAR(D13)</f>
@@ -1748,7 +1904,7 @@
         <v>26310</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:H17" si="2">YEAR(D14)</f>
@@ -1784,7 +1940,7 @@
         <v>19886</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
@@ -1820,7 +1976,7 @@
         <v>11637</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
@@ -1856,7 +2012,7 @@
         <v>36206</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Creacion de script 'data.sql' para poblacion de la DB #12
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
     <sheet name="Address &amp; Admin" sheetId="4" r:id="rId2"/>
     <sheet name="AccountHolder" sheetId="5" r:id="rId3"/>
+    <sheet name="ThirdParty" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="165">
   <si>
     <t>Request Type</t>
   </si>
@@ -317,6 +318,210 @@
   </si>
   <si>
     <t>Admins</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>hashed_key</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Ernesto</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Hernan</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Ramon</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Veronica</t>
+  </si>
+  <si>
+    <t>Ubaldo</t>
+  </si>
+  <si>
+    <t>Wendy</t>
+  </si>
+  <si>
+    <t>Xochil</t>
+  </si>
+  <si>
+    <t>Yolanda</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Liliana</t>
+  </si>
+  <si>
+    <t>Gladys</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>eeee</t>
+  </si>
+  <si>
+    <t>ffff</t>
+  </si>
+  <si>
+    <t>gggg</t>
+  </si>
+  <si>
+    <t>hhhh</t>
+  </si>
+  <si>
+    <t>iiii</t>
+  </si>
+  <si>
+    <t>jjjj</t>
+  </si>
+  <si>
+    <t>kkkk</t>
+  </si>
+  <si>
+    <t>llll</t>
+  </si>
+  <si>
+    <t>mmmm</t>
+  </si>
+  <si>
+    <t>nnnn</t>
+  </si>
+  <si>
+    <t>oooo</t>
+  </si>
+  <si>
+    <t>pppp</t>
+  </si>
+  <si>
+    <t>qqqq</t>
+  </si>
+  <si>
+    <t>rrrr</t>
+  </si>
+  <si>
+    <t>ssss</t>
+  </si>
+  <si>
+    <t>tttt</t>
+  </si>
+  <si>
+    <t>uuuu</t>
+  </si>
+  <si>
+    <t>vvvv</t>
+  </si>
+  <si>
+    <t>wwww</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>yyyy</t>
+  </si>
+  <si>
+    <t>zzzz</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>1960-02-24'</t>
+  </si>
+  <si>
+    <t>1990-03-23'</t>
+  </si>
+  <si>
+    <t>2000-12-12'</t>
+  </si>
+  <si>
+    <t>1998-09-20'</t>
+  </si>
+  <si>
+    <t>1997-12-30'</t>
+  </si>
+  <si>
+    <t>1992-06-10'</t>
+  </si>
+  <si>
+    <t>2001-10-05'</t>
+  </si>
+  <si>
+    <t>1997-04-05'</t>
+  </si>
+  <si>
+    <t>1975-09-13'</t>
+  </si>
+  <si>
+    <t>1984-09-28'</t>
+  </si>
+  <si>
+    <t>1982-12-02'</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>apto 3</t>
   </si>
 </sst>
 </file>
@@ -438,12 +643,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -453,13 +652,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -495,12 +710,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G24" totalsRowShown="0">
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Request Type" dataDxfId="4"/>
+    <tableColumn id="1" name="#" dataDxfId="7"/>
+    <tableColumn id="2" name="Request Type" dataDxfId="6"/>
     <tableColumn id="5" name="Param Type"/>
-    <tableColumn id="7" name="Usuario" dataDxfId="3"/>
+    <tableColumn id="7" name="Usuario" dataDxfId="5"/>
     <tableColumn id="3" name="Endpoint"/>
-    <tableColumn id="4" name="Response Description" dataDxfId="2"/>
+    <tableColumn id="4" name="Response Description" dataDxfId="4"/>
     <tableColumn id="6" name="Requsitos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -514,8 +729,8 @@
     <tableColumn id="2" name="country"/>
     <tableColumn id="3" name="city"/>
     <tableColumn id="4" name="street"/>
-    <tableColumn id="5" name="house_number" dataDxfId="1"/>
-    <tableColumn id="6" name="home_unit" dataDxfId="0"/>
+    <tableColumn id="5" name="house_number" dataDxfId="3"/>
+    <tableColumn id="6" name="home_unit" dataDxfId="2"/>
     <tableColumn id="7" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -528,6 +743,33 @@
     <tableColumn id="1" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:D28" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="name"/>
+    <tableColumn id="2" name="user_id" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="hashed_key"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="H2:I13" totalsRowShown="0" headerRowBorderDxfId="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="street">
+      <calculatedColumnFormula>'Address &amp; Admin'!D4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="house_number">
+      <calculatedColumnFormula>'Address &amp; Admin'!E4</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -812,13 +1054,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1144,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,14 +1401,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1204,10 +1446,10 @@
       <c r="E4" s="3">
         <v>23</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="14" t="str">
+      <c r="I4" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
@@ -1225,10 +1467,10 @@
       <c r="E5" s="3">
         <v>50</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="14" t="str">
+      <c r="I5" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
@@ -1246,10 +1488,10 @@
       <c r="E6" s="3">
         <v>12</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="14" t="str">
+      <c r="I6" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
@@ -1267,10 +1509,10 @@
       <c r="E7" s="3">
         <v>54</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="14" t="str">
+      <c r="I7" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
@@ -1288,10 +1530,10 @@
       <c r="E8" s="3">
         <v>26</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="14" t="str">
+      <c r="I8" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
@@ -1309,10 +1551,10 @@
       <c r="E9" s="3">
         <v>11</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="14" t="str">
+      <c r="I9" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
@@ -1330,10 +1572,10 @@
       <c r="E10" s="3">
         <v>69</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="14" t="str">
+      <c r="I10" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
@@ -1351,10 +1593,12 @@
       <c r="E11" s="3">
         <v>89</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="I11" s="14" t="str">
+      <c r="F11" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
-        <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', '', '' ); </v>
+        <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1370,10 +1614,10 @@
       <c r="E12" s="3">
         <v>24</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="14" t="str">
+      <c r="I12" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
@@ -1391,10 +1635,10 @@
       <c r="E13" s="3">
         <v>48</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="14" t="str">
+      <c r="I13" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
@@ -1412,77 +1656,93 @@
       <c r="E14" s="3">
         <v>33</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G14" t="s">
         <v>90</v>
       </c>
-      <c r="I14" s="14" t="str">
+      <c r="I14" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="14" t="str">
+      <c r="D20" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('John'); </v>
       </c>
       <c r="G20" t="str">
-        <f>CONCATENATE("SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"'; ")</f>
-        <v xml:space="preserve">SELECT user_id FROM users WHERE NAME LIKE 'John'; </v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'John') </v>
+      </c>
+      <c r="I20" t="str">
+        <f>CONCATENATE("INSERT INTO admins VALUES (",G20,"); ")</f>
+        <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="14" t="str">
+      <c r="D21" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alfredo'); </v>
       </c>
       <c r="G21" t="str">
-        <f>CONCATENATE("SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"'; ")</f>
-        <v xml:space="preserve">SELECT user_id FROM users WHERE NAME LIKE 'Alfredo'; </v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') </v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ref="I21:I23" si="0">CONCATENATE("INSERT INTO admins VALUES (",G21,"); ")</f>
+        <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="14" t="str">
+      <c r="D22" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Cristian'); </v>
       </c>
       <c r="G22" t="str">
-        <f>CONCATENATE("SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"'; ")</f>
-        <v xml:space="preserve">SELECT user_id FROM users WHERE NAME LIKE 'Cristian'; </v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Cristian') </v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="14" t="str">
+      <c r="D23" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Raúl'); </v>
       </c>
       <c r="G23" t="str">
-        <f>CONCATENATE("SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"'; ")</f>
-        <v xml:space="preserve">SELECT user_id FROM users WHERE NAME LIKE 'Raúl'; </v>
+        <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Raúl') </v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
       </c>
     </row>
   </sheetData>
@@ -1503,7 +1763,7 @@
   <dimension ref="B3:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,10 +1773,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1633,4 +1893,845 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="12" t="str">
+        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",B3,"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alberto'); </v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" t="str">
+        <f>'Address &amp; Admin'!D4</f>
+        <v>Numancia</v>
+      </c>
+      <c r="I3">
+        <f>'Address &amp; Admin'!E4</f>
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M3" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K3,", ",M3,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') , '1960-02-24', (SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') , null); </v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="12" t="str">
+        <f t="shared" ref="F4:F28" si="0">CONCATENATE("INSERT INTO users (NAME) VALUES ('",B4,"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Bernardo'); </v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" t="str">
+        <f>'Address &amp; Admin'!D5</f>
+        <v>Gran Via</v>
+      </c>
+      <c r="I4">
+        <f>'Address &amp; Admin'!E5</f>
+        <v>50</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M4" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K4,", ",M4,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') , '1990-03-23', (SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') , null); </v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Carlos'); </v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" t="str">
+        <f>'Address &amp; Admin'!D6</f>
+        <v>Napoles</v>
+      </c>
+      <c r="I5">
+        <f>'Address &amp; Admin'!E6</f>
+        <v>12</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M5" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O5" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K5,", ",M5,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') , '2000-12-12', (SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') , null); </v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Daniel'); </v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" t="str">
+        <f>'Address &amp; Admin'!D7</f>
+        <v>Dénia</v>
+      </c>
+      <c r="I6">
+        <f>'Address &amp; Admin'!E7</f>
+        <v>54</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M6" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O6" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K6,", ",M6,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') , '1998-09-20', (SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') , null); </v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ernesto'); </v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" t="str">
+        <f>'Address &amp; Admin'!D8</f>
+        <v>San Blas</v>
+      </c>
+      <c r="I7">
+        <f>'Address &amp; Admin'!E8</f>
+        <v>26</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M7" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O7" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K7,", ",M7,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') , '1997-12-30', (SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') , null); </v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Fernando'); </v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" t="str">
+        <f>'Address &amp; Admin'!D9</f>
+        <v>Rivolí</v>
+      </c>
+      <c r="I8">
+        <f>'Address &amp; Admin'!E9</f>
+        <v>11</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M8" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O8" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K8,", ",M8,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') , '1992-06-10', (SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') , null); </v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Gladys'); </v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" t="str">
+        <f>'Address &amp; Admin'!D10</f>
+        <v>Oberweg</v>
+      </c>
+      <c r="I9">
+        <f>'Address &amp; Admin'!E10</f>
+        <v>69</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M9" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K9,", ",M9,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') , '2001-10-05', (SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') , null); </v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Hernan'); </v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" t="str">
+        <f>'Address &amp; Admin'!D11</f>
+        <v>Av El Dorado</v>
+      </c>
+      <c r="I10">
+        <f>'Address &amp; Admin'!E11</f>
+        <v>89</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O10" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K10,", ",M10,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') , '1997-04-05', (SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') , null); </v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ivan'); </v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" t="str">
+        <f>'Address &amp; Admin'!D12</f>
+        <v>Jirón Callao</v>
+      </c>
+      <c r="I11">
+        <f>'Address &amp; Admin'!E12</f>
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M11" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O11" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K11,", ",M11,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') , '1975-09-13', (SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') , null); </v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Jose'); </v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" t="str">
+        <f>'Address &amp; Admin'!D13</f>
+        <v>Av 9 de Julio</v>
+      </c>
+      <c r="I12">
+        <f>'Address &amp; Admin'!E13</f>
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="M12" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O12" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K12,", ",M12,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Jose') , '1984-09-28', (SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') , null); </v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Kevin'); </v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H13" t="str">
+        <f>'Address &amp; Admin'!D14</f>
+        <v>Paseo de Montejo</v>
+      </c>
+      <c r="I13">
+        <f>'Address &amp; Admin'!E14</f>
+        <v>33</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M13" t="str">
+        <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
+        <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O13" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K13,", ",M13,", ","null","); ")</f>
+        <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') , '1982-12-02', (SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') , null); </v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Liliana') </v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Liliana'); </v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Maria') </v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Maria'); </v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Nancy') </v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Nancy'); </v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Orlando') </v>
+      </c>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Orlando'); </v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Pedro') </v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Pedro'); </v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Quentin') </v>
+      </c>
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Quentin'); </v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ramon') </v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ramon'); </v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
+      </c>
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Samuel'); </v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') , 'ssss'); </v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
+      </c>
+      <c r="D22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Tomas'); </v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') , 'tttt'); </v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
+      </c>
+      <c r="D23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ubaldo'); </v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') , 'uuuu'); </v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
+      </c>
+      <c r="D24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Veronica'); </v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') , 'vvvv'); </v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
+      </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Wendy'); </v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') , 'wwww'); </v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
+      </c>
+      <c r="D26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Xochil'); </v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') , 'xxxx'); </v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
+      </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Yolanda'); </v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') , 'yyyy'); </v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="str">
+        <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
+        <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
+      </c>
+      <c r="D28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Zoe'); </v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H28" s="2" t="str">
+        <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') , 'zzzz'); </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicion de recursos extra #1
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="168">
   <si>
     <t>Request Type</t>
   </si>
@@ -77,33 +77,18 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>/admin</t>
-  </si>
-  <si>
-    <t>/admin/accountholder/{id}</t>
-  </si>
-  <si>
     <t>get info de un account holder</t>
   </si>
   <si>
-    <t>/admin/accountholders</t>
-  </si>
-  <si>
     <t>Bienvenida</t>
   </si>
   <si>
     <t>obtiene listado de todos los accountholders</t>
   </si>
   <si>
-    <t>/admin/accountholders?name={X}</t>
-  </si>
-  <si>
     <t>buscar un account holder por nombre</t>
   </si>
   <si>
-    <t>/admin/accountholders/birthdate?initialdate={X}&amp;finaldate={X}</t>
-  </si>
-  <si>
     <t>mostrar account holders por rango de fechas</t>
   </si>
   <si>
@@ -131,15 +116,9 @@
     <t>Realizar un deposito de fondos</t>
   </si>
   <si>
-    <t>/admin/accountholder/{id}/accounts</t>
-  </si>
-  <si>
     <t>muestra las diversas cuentas de un accountholder</t>
   </si>
   <si>
-    <t>/admin/accountholder/{id}/accounts/{IBAN}</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t>crear un accountholder (Opcional)</t>
   </si>
   <si>
-    <t>crear un ThirdParty user (Opcional)</t>
-  </si>
-  <si>
     <t>PATCH</t>
   </si>
   <si>
@@ -522,6 +498,39 @@
   </si>
   <si>
     <t>apto 3</t>
+  </si>
+  <si>
+    <t>crear un ThirdParty user</t>
+  </si>
+  <si>
+    <t>/admins</t>
+  </si>
+  <si>
+    <t>/admins/</t>
+  </si>
+  <si>
+    <t>/admins/accountholders</t>
+  </si>
+  <si>
+    <t>/admins/accountholder/{id}</t>
+  </si>
+  <si>
+    <t>/admins/accountholders?name={X}</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/birthdate?initialdate={X}&amp;finaldate={X}</t>
+  </si>
+  <si>
+    <t>/admins/accountholder/{id}/accounts</t>
+  </si>
+  <si>
+    <t>/admins/accountholder/{id}/accounts/{IBAN}</t>
+  </si>
+  <si>
+    <t>Bodyrequest</t>
+  </si>
+  <si>
+    <t>Crear nueva cuenta CreditCard</t>
   </si>
 </sst>
 </file>
@@ -708,7 +717,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G24" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G28" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="7"/>
     <tableColumn id="2" name="Request Type" dataDxfId="6"/>
@@ -1036,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,8 +1058,8 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.7109375" customWidth="1"/>
-    <col min="6" max="6" width="103" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="7" max="7" width="49.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
@@ -1082,13 +1091,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1096,115 +1102,64 @@
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>158</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="7" t="s">
-        <v>42</v>
+      <c r="E6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" t="s">
+        <v>157</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
@@ -1214,163 +1169,201 @@
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>36</v>
+      <c r="E12" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>6</v>
-      </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>10</v>
-      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
-      <c r="E20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>11</v>
-      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
-      <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>12</v>
-      </c>
-      <c r="D22" s="5"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>13</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C24">
-      <formula1>"-----,PathVariable,RequestParam"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C28">
+      <formula1>"-----,PathVariable,RequestParam,Bodyrequest"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D28">
       <formula1>"Admin,AccountHolder,ThirdParty"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B28">
       <formula1>"GET,POST,PUT,PATCH,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1402,7 +1395,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -1415,39 +1408,39 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3">
         <v>23</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="I4" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1456,19 +1449,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3">
         <v>50</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="I5" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1477,19 +1470,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3">
         <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I6" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1498,19 +1491,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3">
         <v>54</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I7" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1519,19 +1512,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3">
         <v>26</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="I8" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1540,19 +1533,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3">
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I9" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1561,19 +1554,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E10" s="3">
         <v>69</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I10" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1582,19 +1575,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3">
         <v>89</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I11" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1603,19 +1596,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3">
         <v>24</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I12" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1624,19 +1617,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E13" s="3">
         <v>48</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I13" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1645,22 +1638,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E14" s="3">
         <v>33</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I14" s="12" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
@@ -1669,7 +1662,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1679,7 +1672,7 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D20" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
@@ -1696,7 +1689,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D21" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
@@ -1713,7 +1706,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D22" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
@@ -1730,7 +1723,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D23" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
@@ -1774,10 +1767,10 @@
   <sheetData>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1899,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -1922,38 +1915,38 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F3" s="12" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",B3,"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alberto'); </v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H3" t="str">
         <f>'Address &amp; Admin'!D4</f>
@@ -1964,14 +1957,14 @@
         <v>23</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O3" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K3,", ",M3,", ","null","); ")</f>
@@ -1980,21 +1973,21 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F4" s="12" t="str">
         <f t="shared" ref="F4:F28" si="0">CONCATENATE("INSERT INTO users (NAME) VALUES ('",B4,"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Bernardo'); </v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H4" t="str">
         <f>'Address &amp; Admin'!D5</f>
@@ -2005,14 +1998,14 @@
         <v>50</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O4" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K4,", ",M4,", ","null","); ")</f>
@@ -2021,21 +2014,21 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C5" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F5" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Carlos'); </v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H5" t="str">
         <f>'Address &amp; Admin'!D6</f>
@@ -2046,14 +2039,14 @@
         <v>12</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="M5" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O5" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K5,", ",M5,", ","null","); ")</f>
@@ -2062,21 +2055,21 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C6" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F6" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Daniel'); </v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H6" t="str">
         <f>'Address &amp; Admin'!D7</f>
@@ -2087,14 +2080,14 @@
         <v>54</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="M6" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O6" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K6,", ",M6,", ","null","); ")</f>
@@ -2103,21 +2096,21 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C7" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F7" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ernesto'); </v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H7" t="str">
         <f>'Address &amp; Admin'!D8</f>
@@ -2128,14 +2121,14 @@
         <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="M7" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O7" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K7,", ",M7,", ","null","); ")</f>
@@ -2144,21 +2137,21 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F8" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Fernando'); </v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H8" t="str">
         <f>'Address &amp; Admin'!D9</f>
@@ -2169,14 +2162,14 @@
         <v>11</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="M8" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O8" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K8,", ",M8,", ","null","); ")</f>
@@ -2185,21 +2178,21 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C9" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F9" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Gladys'); </v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H9" t="str">
         <f>'Address &amp; Admin'!D10</f>
@@ -2210,14 +2203,14 @@
         <v>69</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="M9" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O9" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K9,", ",M9,", ","null","); ")</f>
@@ -2226,21 +2219,21 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F10" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Hernan'); </v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H10" t="str">
         <f>'Address &amp; Admin'!D11</f>
@@ -2251,14 +2244,14 @@
         <v>89</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="M10" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O10" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K10,", ",M10,", ","null","); ")</f>
@@ -2267,21 +2260,21 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C11" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F11" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ivan'); </v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H11" t="str">
         <f>'Address &amp; Admin'!D12</f>
@@ -2292,14 +2285,14 @@
         <v>24</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="M11" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O11" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K11,", ",M11,", ","null","); ")</f>
@@ -2308,21 +2301,21 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C12" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F12" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Jose'); </v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H12" t="str">
         <f>'Address &amp; Admin'!D13</f>
@@ -2333,14 +2326,14 @@
         <v>48</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="M12" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O12" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K12,", ",M12,", ","null","); ")</f>
@@ -2349,21 +2342,21 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C13" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F13" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Kevin'); </v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H13" t="str">
         <f>'Address &amp; Admin'!D14</f>
@@ -2374,14 +2367,14 @@
         <v>33</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="M13" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O13" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K13,", ",M13,", ","null","); ")</f>
@@ -2390,175 +2383,175 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Liliana') </v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F14" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Liliana'); </v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Maria') </v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F15" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Maria'); </v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Nancy') </v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F16" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Nancy'); </v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Orlando') </v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F17" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Orlando'); </v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Pedro') </v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F18" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Pedro'); </v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Quentin') </v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F19" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Quentin'); </v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ramon') </v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F20" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ramon'); </v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F21" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Samuel'); </v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H21" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2567,21 +2560,21 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F22" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Tomas'); </v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H22" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2590,21 +2583,21 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F23" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ubaldo'); </v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H23" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2613,21 +2606,21 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C24" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F24" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Veronica'); </v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H24" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2636,21 +2629,21 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
       </c>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F25" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Wendy'); </v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H25" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2659,21 +2652,21 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F26" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Xochil'); </v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H26" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2682,21 +2675,21 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C27" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F27" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Yolanda'); </v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H27" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2705,21 +2698,21 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C28" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F28" s="12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Zoe'); </v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H28" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>

</xml_diff>

<commit_message>
Modificaciones a las definiciones de los endpoints y a los requerimientos.
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="181">
   <si>
     <t>Request Type</t>
   </si>
@@ -44,9 +44,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>/doctors</t>
-  </si>
-  <si>
     <t>Param Type</t>
   </si>
   <si>
@@ -56,15 +53,6 @@
     <t>RequestParam</t>
   </si>
   <si>
-    <t>/patients/{id}</t>
-  </si>
-  <si>
-    <t>/doctors/{id}?status={X}</t>
-  </si>
-  <si>
-    <t>/doctors/{id}?department={X}</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -95,42 +83,18 @@
     <t>AccountHolder</t>
   </si>
   <si>
-    <t>/accountholder</t>
-  </si>
-  <si>
     <t>Muestra todas sus cuentas</t>
   </si>
   <si>
-    <t>/accountholder/{iban}</t>
-  </si>
-  <si>
     <t>Muestra el detalle de una especifica cuenta.</t>
   </si>
   <si>
-    <t>/accountholder/{iban}/withdraw</t>
-  </si>
-  <si>
-    <t>Solicitar un retiro de fondos</t>
-  </si>
-  <si>
-    <t>Realizar un deposito de fondos</t>
-  </si>
-  <si>
     <t>muestra las diversas cuentas de un accountholder</t>
   </si>
   <si>
     <t>POST</t>
   </si>
   <si>
-    <t>Requsitos</t>
-  </si>
-  <si>
-    <t>Type, name, birthdate, address 1, address 2</t>
-  </si>
-  <si>
-    <t>Type, name, hashedKey</t>
-  </si>
-  <si>
     <t>crear un accountholder (Opcional)</t>
   </si>
   <si>
@@ -140,9 +104,6 @@
     <t>Modifica el saldo de la cuenta indicada</t>
   </si>
   <si>
-    <t>IBAN, nuevo saldo</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -506,31 +467,109 @@
     <t>/admins</t>
   </si>
   <si>
-    <t>/admins/</t>
-  </si>
-  <si>
     <t>/admins/accountholders</t>
   </si>
   <si>
-    <t>/admins/accountholder/{id}</t>
-  </si>
-  <si>
     <t>/admins/accountholders?name={X}</t>
   </si>
   <si>
     <t>/admins/accountholders/birthdate?initialdate={X}&amp;finaldate={X}</t>
   </si>
   <si>
-    <t>/admins/accountholder/{id}/accounts</t>
-  </si>
-  <si>
-    <t>/admins/accountholder/{id}/accounts/{IBAN}</t>
-  </si>
-  <si>
     <t>Bodyrequest</t>
   </si>
   <si>
     <t>Crear nueva cuenta CreditCard</t>
+  </si>
+  <si>
+    <t>UserType, name, birthdate, address 1, address 2</t>
+  </si>
+  <si>
+    <t>UserType, name, hashedKey</t>
+  </si>
+  <si>
+    <t>AccountType, owner1, owner2, amount, penalty fee, interes rate</t>
+  </si>
+  <si>
+    <t>Crear nueva cuenta Saving</t>
+  </si>
+  <si>
+    <t>Crear nueva cuenta Checking</t>
+  </si>
+  <si>
+    <t>AccountType, owner1, owner2, amount, penalty fee, interes rate, secret key, minimumBalance, status</t>
+  </si>
+  <si>
+    <t>AccountType, owner1, owner2, amount, penalty fee, secret key, minimumBalance, monthlyMaintenanceFee, status</t>
+  </si>
+  <si>
+    <t>Crear nueva cuenta StudentChecking</t>
+  </si>
+  <si>
+    <t>AccountType, owner1, owner2, amount, penalty fee, secret key, status</t>
+  </si>
+  <si>
+    <t>Requsitos o Respuesta</t>
+  </si>
+  <si>
+    <t>TODOS en detalle</t>
+  </si>
+  <si>
+    <t>Name, birthdate, address 1 , address 2</t>
+  </si>
+  <si>
+    <t>Cantidad y tipo de cuentas que tiene ese usuario.</t>
+  </si>
+  <si>
+    <t>IBAN, anterior saldo, nuevo saldo</t>
+  </si>
+  <si>
+    <t>Crea una det. Cuenta al usuario en cuestion.</t>
+  </si>
+  <si>
+    <t>accountType, owner2 ?, account data body.</t>
+  </si>
+  <si>
+    <t>/accountholder/{id}</t>
+  </si>
+  <si>
+    <t>/accountholder/{id}/{IBAN}</t>
+  </si>
+  <si>
+    <t>/accountholder/{id}/{IBAN}?transaction={X}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar transferencia </t>
+  </si>
+  <si>
+    <t>ThirdParty</t>
+  </si>
+  <si>
+    <t>Enviar o recibir dinero.</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>transactionType, thirdParty name, IBAN, amount, secret key</t>
+  </si>
+  <si>
+    <t>/thirdparty?transactionType={X}</t>
+  </si>
+  <si>
+    <t>transactionType, name owner1 OR owner2, IBAN, amount</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}/accounts</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}/accounts/{IBAN}</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}?accountType={X}</t>
   </si>
 </sst>
 </file>
@@ -633,7 +672,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -648,7 +687,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -661,12 +699,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
@@ -717,7 +764,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G28" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G25" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="7"/>
     <tableColumn id="2" name="Request Type" dataDxfId="6"/>
@@ -725,7 +772,7 @@
     <tableColumn id="7" name="Usuario" dataDxfId="5"/>
     <tableColumn id="3" name="Endpoint"/>
     <tableColumn id="4" name="Response Description" dataDxfId="4"/>
-    <tableColumn id="6" name="Requsitos"/>
+    <tableColumn id="6" name="Requsitos o Respuesta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1045,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G28"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,17 +1106,17 @@
     <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.7109375" customWidth="1"/>
     <col min="6" max="6" width="53.5703125" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1079,10 +1126,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>
@@ -1091,105 +1138,116 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>158</v>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="7" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>167</v>
+        <v>150</v>
+      </c>
+      <c r="G7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D11"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>161</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1197,16 +1255,19 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>162</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,30 +1275,33 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1245,41 +1309,65 @@
         <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>165</v>
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="5"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="5"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
@@ -1287,83 +1375,84 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="5"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>170</v>
+      </c>
+      <c r="G23" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
-      <c r="E24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="5"/>
+      <c r="B25" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="E25" s="2" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="5"/>
-      <c r="E26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
-      <c r="E27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="5"/>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="G25" t="s">
+        <v>174</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C25">
       <formula1>"-----,PathVariable,RequestParam,Bodyrequest"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D25">
       <formula1>"Admin,AccountHolder,ThirdParty"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B25">
       <formula1>"GET,POST,PUT,PATCH,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1394,287 +1483,287 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E4" s="3">
         <v>23</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="12" t="str">
+      <c r="F4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3">
         <v>50</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="12" t="str">
+      <c r="F5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3">
         <v>12</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="12" t="str">
+      <c r="F6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3">
         <v>54</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="12" t="str">
+      <c r="F7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3">
         <v>26</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="12" t="str">
+      <c r="F8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3">
         <v>11</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="12" t="str">
+      <c r="F9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3">
         <v>69</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="12" t="str">
+      <c r="F10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3">
         <v>89</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="I11" s="12" t="str">
+      <c r="F11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3">
         <v>24</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="12" t="str">
+      <c r="F12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3">
         <v>48</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="12" t="str">
+      <c r="F13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3">
         <v>33</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>81</v>
+      <c r="F14" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="12" t="str">
+        <v>69</v>
+      </c>
+      <c r="I14" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>88</v>
+      <c r="B18" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="12" t="str">
+        <v>71</v>
+      </c>
+      <c r="D20" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('John'); </v>
       </c>
@@ -1689,9 +1778,9 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="12" t="str">
+        <v>72</v>
+      </c>
+      <c r="D21" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alfredo'); </v>
       </c>
@@ -1706,9 +1795,9 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="12" t="str">
+        <v>73</v>
+      </c>
+      <c r="D22" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Cristian'); </v>
       </c>
@@ -1723,9 +1812,9 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="12" t="str">
+        <v>74</v>
+      </c>
+      <c r="D23" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Raúl'); </v>
       </c>
@@ -1766,11 +1855,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>41</v>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1912,41 +2001,41 @@
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>41</v>
+        <v>77</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="12" t="str">
+        <v>103</v>
+      </c>
+      <c r="F3" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",B3,"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alberto'); </v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H3" t="str">
         <f>'Address &amp; Admin'!D4</f>
@@ -1957,14 +2046,14 @@
         <v>23</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O3" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K3,", ",M3,", ","null","); ")</f>
@@ -1973,21 +2062,21 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" s="12" t="str">
+        <v>104</v>
+      </c>
+      <c r="F4" s="11" t="str">
         <f t="shared" ref="F4:F28" si="0">CONCATENATE("INSERT INTO users (NAME) VALUES ('",B4,"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Bernardo'); </v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H4" t="str">
         <f>'Address &amp; Admin'!D5</f>
@@ -1998,14 +2087,14 @@
         <v>50</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O4" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K4,", ",M4,", ","null","); ")</f>
@@ -2014,21 +2103,21 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C5" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="12" t="str">
+        <v>105</v>
+      </c>
+      <c r="F5" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Carlos'); </v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H5" t="str">
         <f>'Address &amp; Admin'!D6</f>
@@ -2039,14 +2128,14 @@
         <v>12</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="M5" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O5" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K5,", ",M5,", ","null","); ")</f>
@@ -2055,21 +2144,21 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C6" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F6" s="12" t="str">
+        <v>106</v>
+      </c>
+      <c r="F6" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Daniel'); </v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H6" t="str">
         <f>'Address &amp; Admin'!D7</f>
@@ -2080,14 +2169,14 @@
         <v>54</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="M6" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O6" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K6,", ",M6,", ","null","); ")</f>
@@ -2096,21 +2185,21 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C7" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="12" t="str">
+        <v>107</v>
+      </c>
+      <c r="F7" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ernesto'); </v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H7" t="str">
         <f>'Address &amp; Admin'!D8</f>
@@ -2121,14 +2210,14 @@
         <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="M7" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O7" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K7,", ",M7,", ","null","); ")</f>
@@ -2137,21 +2226,21 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="12" t="str">
+        <v>108</v>
+      </c>
+      <c r="F8" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Fernando'); </v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H8" t="str">
         <f>'Address &amp; Admin'!D9</f>
@@ -2162,14 +2251,14 @@
         <v>11</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="M8" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O8" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K8,", ",M8,", ","null","); ")</f>
@@ -2178,21 +2267,21 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C9" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="12" t="str">
+        <v>109</v>
+      </c>
+      <c r="F9" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Gladys'); </v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H9" t="str">
         <f>'Address &amp; Admin'!D10</f>
@@ -2203,14 +2292,14 @@
         <v>69</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="M9" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O9" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K9,", ",M9,", ","null","); ")</f>
@@ -2219,21 +2308,21 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="12" t="str">
+        <v>110</v>
+      </c>
+      <c r="F10" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Hernan'); </v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H10" t="str">
         <f>'Address &amp; Admin'!D11</f>
@@ -2244,14 +2333,14 @@
         <v>89</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="M10" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O10" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K10,", ",M10,", ","null","); ")</f>
@@ -2260,21 +2349,21 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C11" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="12" t="str">
+        <v>111</v>
+      </c>
+      <c r="F11" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ivan'); </v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H11" t="str">
         <f>'Address &amp; Admin'!D12</f>
@@ -2285,14 +2374,14 @@
         <v>24</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="M11" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O11" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K11,", ",M11,", ","null","); ")</f>
@@ -2301,21 +2390,21 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C12" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" s="12" t="str">
+        <v>112</v>
+      </c>
+      <c r="F12" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Jose'); </v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H12" t="str">
         <f>'Address &amp; Admin'!D13</f>
@@ -2326,14 +2415,14 @@
         <v>48</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="M12" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O12" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K12,", ",M12,", ","null","); ")</f>
@@ -2342,21 +2431,21 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C13" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="12" t="str">
+        <v>113</v>
+      </c>
+      <c r="F13" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Kevin'); </v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H13" t="str">
         <f>'Address &amp; Admin'!D14</f>
@@ -2367,14 +2456,14 @@
         <v>33</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="M13" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O13" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, address_address_id, mailing_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K13,", ",M13,", ","null","); ")</f>
@@ -2383,175 +2472,175 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Liliana') </v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" s="12" t="str">
+        <v>114</v>
+      </c>
+      <c r="F14" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Liliana'); </v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Maria') </v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="12" t="str">
+        <v>115</v>
+      </c>
+      <c r="F15" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Maria'); </v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Nancy') </v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="12" t="str">
+        <v>116</v>
+      </c>
+      <c r="F16" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Nancy'); </v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Orlando') </v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="12" t="str">
+        <v>117</v>
+      </c>
+      <c r="F17" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Orlando'); </v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Pedro') </v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="12" t="str">
+        <v>118</v>
+      </c>
+      <c r="F18" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Pedro'); </v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Quentin') </v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="12" t="str">
+        <v>119</v>
+      </c>
+      <c r="F19" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Quentin'); </v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ramon') </v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="12" t="str">
+        <v>120</v>
+      </c>
+      <c r="F20" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ramon'); </v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
       </c>
       <c r="D21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="12" t="str">
+        <v>121</v>
+      </c>
+      <c r="F21" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Samuel'); </v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H21" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2560,21 +2649,21 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="12" t="str">
+        <v>122</v>
+      </c>
+      <c r="F22" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Tomas'); </v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H22" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2583,21 +2672,21 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
-      </c>
-      <c r="F23" s="12" t="str">
+        <v>123</v>
+      </c>
+      <c r="F23" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ubaldo'); </v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H23" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2606,21 +2695,21 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C24" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F24" s="12" t="str">
+        <v>124</v>
+      </c>
+      <c r="F24" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Veronica'); </v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H24" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2629,21 +2718,21 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
       </c>
       <c r="D25" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="12" t="str">
+        <v>125</v>
+      </c>
+      <c r="F25" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Wendy'); </v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H25" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2652,21 +2741,21 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="12" t="str">
+        <v>126</v>
+      </c>
+      <c r="F26" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Xochil'); </v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H26" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2675,21 +2764,21 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C27" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="12" t="str">
+        <v>127</v>
+      </c>
+      <c r="F27" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Yolanda'); </v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H27" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
@@ -2698,21 +2787,21 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C28" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="12" t="str">
+        <v>128</v>
+      </c>
+      <c r="F28" s="11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Zoe'); </v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H28" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>

</xml_diff>

<commit_message>
Changes and updates about the progress and development of the project. #1
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="188">
   <si>
     <t>Request Type</t>
   </si>
@@ -515,12 +515,6 @@
     <t>IBAN, anterior saldo, nuevo saldo</t>
   </si>
   <si>
-    <t>Crea una det. Cuenta al usuario en cuestion.</t>
-  </si>
-  <si>
-    <t>accountType, owner2 ?, account data body.</t>
-  </si>
-  <si>
     <t>/accountholder/{id}</t>
   </si>
   <si>
@@ -560,9 +554,6 @@
     <t>/admins/accountholders/{id}/accounts/{IBAN}</t>
   </si>
   <si>
-    <t>/admins/accountholders/{id}?accountType={X}</t>
-  </si>
-  <si>
     <t>name, birthdate, address 1, address 2</t>
   </si>
   <si>
@@ -576,13 +567,37 @@
   </si>
   <si>
     <t>crear un accountholder</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}/newchecking</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}/newsavings</t>
+  </si>
+  <si>
+    <t>/admins/accountholders/{id}/newcreditcard</t>
+  </si>
+  <si>
+    <t>Crea una nueva cuenta de tipo checking al usuario.</t>
+  </si>
+  <si>
+    <t>Crea una nueva cuenta de tipo savings al usuario.</t>
+  </si>
+  <si>
+    <t>Crea una nueva cuenta de tipo creditcard al usuario.</t>
+  </si>
+  <si>
+    <t>owner2 ?, account data body.</t>
+  </si>
+  <si>
+    <t>Owner2?, Money(currency, amount), Secret key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,8 +635,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,6 +672,11 @@
         <bgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -673,12 +700,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -710,18 +738,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -769,7 +799,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G28" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="7"/>
     <tableColumn id="2" name="Request Type" dataDxfId="6"/>
@@ -1097,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,13 +1145,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1168,13 +1198,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1188,13 +1218,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F6" t="s">
         <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1242,7 +1272,7 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -1262,11 +1292,11 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
@@ -1282,7 +1312,7 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="14" t="s">
@@ -1299,7 +1329,7 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="14" t="s">
@@ -1317,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>20</v>
@@ -1334,7 +1364,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>19</v>
@@ -1348,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
@@ -1361,89 +1391,125 @@
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>177</v>
+      <c r="E19" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="G19" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G20" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" t="s">
         <v>169</v>
-      </c>
-      <c r="G25" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1451,13 +1517,13 @@
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C28">
       <formula1>"-----,PathVariable,RequestParam,Bodyrequest"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D28">
       <formula1>"Admin,AccountHolder,ThirdParty"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B28">
       <formula1>"GET,POST,PUT,PATCH,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1488,14 +1554,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
modified the size of the password field in the inserts. #12
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="191">
   <si>
     <t>Request Type</t>
   </si>
@@ -591,6 +591,15 @@
   </si>
   <si>
     <t>Owner2?, Money(currency, amount), Secret key</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -741,13 +750,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
@@ -755,7 +764,19 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thick">
@@ -801,12 +822,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G28" totalsRowShown="0">
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="7"/>
-    <tableColumn id="2" name="Request Type" dataDxfId="6"/>
+    <tableColumn id="1" name="#" dataDxfId="11"/>
+    <tableColumn id="2" name="Request Type" dataDxfId="10"/>
     <tableColumn id="5" name="Param Type"/>
-    <tableColumn id="7" name="Usuario" dataDxfId="5"/>
+    <tableColumn id="7" name="Usuario" dataDxfId="9"/>
     <tableColumn id="3" name="Endpoint"/>
-    <tableColumn id="4" name="Response Description" dataDxfId="4"/>
+    <tableColumn id="4" name="Response Description" dataDxfId="8"/>
     <tableColumn id="6" name="Requsitos o Respuesta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -820,8 +841,8 @@
     <tableColumn id="2" name="country"/>
     <tableColumn id="3" name="city"/>
     <tableColumn id="4" name="street"/>
-    <tableColumn id="5" name="house_number" dataDxfId="3"/>
-    <tableColumn id="6" name="home_unit" dataDxfId="2"/>
+    <tableColumn id="5" name="house_number" dataDxfId="7"/>
+    <tableColumn id="6" name="home_unit" dataDxfId="6"/>
     <tableColumn id="7" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -829,19 +850,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B19:B23" totalsRowShown="0">
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B19:E23" totalsRowShown="0">
+  <tableColumns count="4">
     <tableColumn id="1" name="name"/>
+    <tableColumn id="2" name="username" dataDxfId="2">
+      <calculatedColumnFormula>LOWER(Tabla3[[#This Row],[name]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="email" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="password"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:D28" totalsRowShown="0">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:G28" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" name="name"/>
-    <tableColumn id="2" name="user_id" dataDxfId="1">
+    <tableColumn id="5" name="username" dataDxfId="3">
+      <calculatedColumnFormula>LOWER(Tabla4[[#This Row],[name]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="email" dataDxfId="0">
+      <calculatedColumnFormula>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="password"/>
+    <tableColumn id="2" name="user_id" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="hashed_key"/>
@@ -851,7 +886,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="H2:I13" totalsRowShown="0" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="K2:L13" totalsRowShown="0" headerRowBorderDxfId="4">
   <tableColumns count="2">
     <tableColumn id="1" name="street">
       <calculatedColumnFormula>'Address &amp; Admin'!D4</calculatedColumnFormula>
@@ -1129,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1145,13 +1180,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1428,7 +1463,7 @@
       <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>182</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1537,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G20" sqref="G20:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,14 +1589,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1820,80 +1855,145 @@
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="11" t="str">
-        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('John'); </v>
-      </c>
-      <c r="G20" t="str">
+      <c r="C20" t="str">
+        <f>LOWER(Tabla3[[#This Row],[name]])</f>
+        <v>john</v>
+      </c>
+      <c r="D20" t="str">
+        <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
+        <v>john@email.com</v>
+      </c>
+      <c r="E20">
+        <v>123456</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '123456'); </v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'John') </v>
       </c>
-      <c r="I20" t="str">
-        <f>CONCATENATE("INSERT INTO admins VALUES (",G20,"); ")</f>
+      <c r="L20" t="str">
+        <f>CONCATENATE("INSERT INTO admins VALUES (",J20,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="11" t="str">
-        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alfredo'); </v>
-      </c>
-      <c r="G21" t="str">
+      <c r="C21" t="str">
+        <f>LOWER(Tabla3[[#This Row],[name]])</f>
+        <v>alfredo</v>
+      </c>
+      <c r="D21" t="str">
+        <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
+        <v>alfredo@email.com</v>
+      </c>
+      <c r="E21">
+        <v>123456</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '123456'); </v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') </v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" ref="I21:I23" si="0">CONCATENATE("INSERT INTO admins VALUES (",G21,"); ")</f>
+      <c r="L21" t="str">
+        <f t="shared" ref="L21:L23" si="0">CONCATENATE("INSERT INTO admins VALUES (",J21,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="11" t="str">
-        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Cristian'); </v>
-      </c>
-      <c r="G22" t="str">
+      <c r="C22" t="str">
+        <f>LOWER(Tabla3[[#This Row],[name]])</f>
+        <v>cristian</v>
+      </c>
+      <c r="D22" t="str">
+        <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
+        <v>cristian@email.com</v>
+      </c>
+      <c r="E22">
+        <v>123456</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '123456'); </v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Cristian') </v>
       </c>
-      <c r="I22" t="str">
+      <c r="L22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="11" t="str">
-        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",Tabla3[[#This Row],[name]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Raúl'); </v>
-      </c>
-      <c r="G23" t="str">
+      <c r="C23" t="str">
+        <f>LOWER(Tabla3[[#This Row],[name]])</f>
+        <v>raúl</v>
+      </c>
+      <c r="D23" t="str">
+        <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
+        <v>raúl@email.com</v>
+      </c>
+      <c r="E23">
+        <v>123456</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '123456'); </v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Raúl') </v>
       </c>
-      <c r="I23" t="str">
+      <c r="L23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
       </c>
@@ -2050,833 +2150,1146 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O28"/>
+  <dimension ref="B2:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>alberto</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>alberto@email.com</v>
+      </c>
+      <c r="E3">
+        <v>123456</v>
+      </c>
+      <c r="F3" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="11" t="str">
-        <f>CONCATENATE("INSERT INTO users (NAME) VALUES ('",B3,"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Alberto'); </v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H3" t="str">
+      <c r="I3" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B3,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alberto', 'alberto', 'alberto@email.com', '123456'); </v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" t="str">
         <f>'Address &amp; Admin'!D4</f>
         <v>Numancia</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <f>'Address &amp; Admin'!E4</f>
         <v>23</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="M3" t="str">
+      <c r="P3" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O3" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K3,", ",M3,", ","null","); ")</f>
+      <c r="Q3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R3" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N3,", ",P3,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') , '1960-02-24', (SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') , null); </v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>bernardo</v>
+      </c>
+      <c r="D4" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>bernardo@email.com</v>
+      </c>
+      <c r="E4">
+        <v>123456</v>
+      </c>
+      <c r="F4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="11" t="str">
-        <f t="shared" ref="F4:F28" si="0">CONCATENATE("INSERT INTO users (NAME) VALUES ('",B4,"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Bernardo'); </v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" t="str">
+      <c r="I4" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B4,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Bernardo', 'bernardo', 'bernardo@email.com', '123456'); </v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" t="str">
         <f>'Address &amp; Admin'!D5</f>
         <v>Gran Via</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <f>'Address &amp; Admin'!E5</f>
         <v>50</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M4" t="str">
+      <c r="P4" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O4" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K4,", ",M4,", ","null","); ")</f>
+      <c r="Q4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R4" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N4,", ",P4,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') , '1990-03-23', (SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') , null); </v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>79</v>
       </c>
       <c r="C5" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>carlos</v>
+      </c>
+      <c r="D5" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>carlos@email.com</v>
+      </c>
+      <c r="E5">
+        <v>123456</v>
+      </c>
+      <c r="F5" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Carlos'); </v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" t="str">
+      <c r="I5" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B5,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Carlos', 'carlos', 'carlos@email.com', '123456'); </v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" t="str">
         <f>'Address &amp; Admin'!D6</f>
         <v>Napoles</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <f>'Address &amp; Admin'!E6</f>
         <v>12</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M5" t="str">
+      <c r="P5" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O5" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K5,", ",M5,", ","null","); ")</f>
+      <c r="Q5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R5" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N5,", ",P5,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') , '2000-12-12', (SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') , null); </v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>80</v>
       </c>
       <c r="C6" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>daniel</v>
+      </c>
+      <c r="D6" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>daniel@email.com</v>
+      </c>
+      <c r="E6">
+        <v>123456</v>
+      </c>
+      <c r="F6" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Daniel'); </v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" t="str">
+      <c r="I6" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B6,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Daniel', 'daniel', 'daniel@email.com', '123456'); </v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" t="str">
         <f>'Address &amp; Admin'!D7</f>
         <v>Dénia</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <f>'Address &amp; Admin'!E7</f>
         <v>54</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M6" t="str">
+      <c r="P6" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O6" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K6,", ",M6,", ","null","); ")</f>
+      <c r="Q6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R6" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N6,", ",P6,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') , '1998-09-20', (SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') , null); </v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>81</v>
       </c>
       <c r="C7" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>ernesto</v>
+      </c>
+      <c r="D7" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>ernesto@email.com</v>
+      </c>
+      <c r="E7">
+        <v>123456</v>
+      </c>
+      <c r="F7" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ernesto'); </v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" t="str">
+      <c r="I7" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B7,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ernesto', 'ernesto', 'ernesto@email.com', '123456'); </v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="str">
         <f>'Address &amp; Admin'!D8</f>
         <v>San Blas</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <f>'Address &amp; Admin'!E8</f>
         <v>26</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M7" t="str">
+      <c r="P7" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O7" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K7,", ",M7,", ","null","); ")</f>
+      <c r="Q7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R7" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N7,", ",P7,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') , '1997-12-30', (SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') , null); </v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>82</v>
       </c>
       <c r="C8" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>fernando</v>
+      </c>
+      <c r="D8" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>fernando@email.com</v>
+      </c>
+      <c r="E8">
+        <v>123456</v>
+      </c>
+      <c r="F8" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Fernando'); </v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" t="str">
+      <c r="I8" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B8,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Fernando', 'fernando', 'fernando@email.com', '123456'); </v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" t="str">
         <f>'Address &amp; Admin'!D9</f>
         <v>Rivolí</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <f>'Address &amp; Admin'!E9</f>
         <v>11</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M8" t="str">
+      <c r="P8" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O8" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K8,", ",M8,", ","null","); ")</f>
+      <c r="Q8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R8" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N8,", ",P8,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') , '1992-06-10', (SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') , null); </v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>100</v>
       </c>
       <c r="C9" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>gladys</v>
+      </c>
+      <c r="D9" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>gladys@email.com</v>
+      </c>
+      <c r="E9">
+        <v>123456</v>
+      </c>
+      <c r="F9" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Gladys'); </v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H9" t="str">
+      <c r="I9" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B9,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Gladys', 'gladys', 'gladys@email.com', '123456'); </v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" t="str">
         <f>'Address &amp; Admin'!D10</f>
         <v>Oberweg</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <f>'Address &amp; Admin'!E10</f>
         <v>69</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M9" t="str">
+      <c r="P9" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O9" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K9,", ",M9,", ","null","); ")</f>
+      <c r="Q9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R9" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N9,", ",P9,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') , '2001-10-05', (SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') , null); </v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>83</v>
       </c>
       <c r="C10" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>hernan</v>
+      </c>
+      <c r="D10" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>hernan@email.com</v>
+      </c>
+      <c r="E10">
+        <v>123456</v>
+      </c>
+      <c r="F10" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Hernan'); </v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H10" t="str">
+      <c r="I10" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B10,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Hernan', 'hernan', 'hernan@email.com', '123456'); </v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" t="str">
         <f>'Address &amp; Admin'!D11</f>
         <v>Av El Dorado</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <f>'Address &amp; Admin'!E11</f>
         <v>89</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M10" t="str">
+      <c r="P10" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O10" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K10,", ",M10,", ","null","); ")</f>
+      <c r="Q10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R10" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N10,", ",P10,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') , '1997-04-05', (SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') , null); </v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>84</v>
       </c>
       <c r="C11" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>ivan</v>
+      </c>
+      <c r="D11" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>ivan@email.com</v>
+      </c>
+      <c r="E11">
+        <v>123456</v>
+      </c>
+      <c r="F11" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ivan'); </v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" t="str">
+      <c r="I11" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B11,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ivan', 'ivan', 'ivan@email.com', '123456'); </v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" t="str">
         <f>'Address &amp; Admin'!D12</f>
         <v>Jirón Callao</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <f>'Address &amp; Admin'!E12</f>
         <v>24</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M11" t="str">
+      <c r="P11" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O11" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K11,", ",M11,", ","null","); ")</f>
+      <c r="Q11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R11" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N11,", ",P11,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') , '1975-09-13', (SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') , null); </v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>85</v>
       </c>
       <c r="C12" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>jose</v>
+      </c>
+      <c r="D12" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>jose@email.com</v>
+      </c>
+      <c r="E12">
+        <v>123456</v>
+      </c>
+      <c r="F12" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Jose'); </v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" t="str">
+      <c r="I12" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B12,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Jose', 'jose', 'jose@email.com', '123456'); </v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K12" t="str">
         <f>'Address &amp; Admin'!D13</f>
         <v>Av 9 de Julio</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <f>'Address &amp; Admin'!E13</f>
         <v>48</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M12" t="str">
+      <c r="P12" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O12" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K12,", ",M12,", ","null","); ")</f>
+      <c r="Q12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R12" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N12,", ",P12,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Jose') , '1984-09-28', (SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') , null); </v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>86</v>
       </c>
       <c r="C13" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>kevin</v>
+      </c>
+      <c r="D13" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>kevin@email.com</v>
+      </c>
+      <c r="E13">
+        <v>123456</v>
+      </c>
+      <c r="F13" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Kevin'); </v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" t="str">
+      <c r="I13" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B13,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Kevin', 'kevin', 'kevin@email.com', '123456'); </v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K13" t="str">
         <f>'Address &amp; Admin'!D14</f>
         <v>Paseo de Montejo</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <f>'Address &amp; Admin'!E14</f>
         <v>33</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="M13" t="str">
+      <c r="P13" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O13" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",K13,", ",M13,", ","null","); ")</f>
+      <c r="Q13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R13" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N13,", ",P13,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') , '1982-12-02', (SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') , null); </v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>99</v>
       </c>
       <c r="C14" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>liliana</v>
+      </c>
+      <c r="D14" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>liliana@email.com</v>
+      </c>
+      <c r="E14">
+        <v>123456</v>
+      </c>
+      <c r="F14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Liliana') </v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Liliana'); </v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I14" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B14,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Liliana', 'liliana', 'liliana@email.com', '123456'); </v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>98</v>
       </c>
       <c r="C15" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>maria</v>
+      </c>
+      <c r="D15" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>maria@email.com</v>
+      </c>
+      <c r="E15">
+        <v>123456</v>
+      </c>
+      <c r="F15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Maria') </v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Maria'); </v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I15" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B15,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Maria', 'maria', 'maria@email.com', '123456'); </v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>128</v>
       </c>
       <c r="C16" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>nancy</v>
+      </c>
+      <c r="D16" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>nancy@email.com</v>
+      </c>
+      <c r="E16">
+        <v>123456</v>
+      </c>
+      <c r="F16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Nancy') </v>
       </c>
-      <c r="D16" t="s">
+      <c r="G16" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Nancy'); </v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I16" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B16,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Nancy', 'nancy', 'nancy@email.com', '123456'); </v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>87</v>
       </c>
       <c r="C17" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>orlando</v>
+      </c>
+      <c r="D17" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>orlando@email.com</v>
+      </c>
+      <c r="E17">
+        <v>123456</v>
+      </c>
+      <c r="F17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Orlando') </v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Orlando'); </v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I17" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B17,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Orlando', 'orlando', 'orlando@email.com', '123456'); </v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>88</v>
       </c>
       <c r="C18" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>pedro</v>
+      </c>
+      <c r="D18" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>pedro@email.com</v>
+      </c>
+      <c r="E18">
+        <v>123456</v>
+      </c>
+      <c r="F18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Pedro') </v>
       </c>
-      <c r="D18" t="s">
+      <c r="G18" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Pedro'); </v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I18" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B18,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Pedro', 'pedro', 'pedro@email.com', '123456'); </v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>101</v>
       </c>
       <c r="C19" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>quentin</v>
+      </c>
+      <c r="D19" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>quentin@email.com</v>
+      </c>
+      <c r="E19">
+        <v>123456</v>
+      </c>
+      <c r="F19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Quentin') </v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Quentin'); </v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I19" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B19,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Quentin', 'quentin', 'quentin@email.com', '123456'); </v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>ramon</v>
+      </c>
+      <c r="D20" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>ramon@email.com</v>
+      </c>
+      <c r="E20">
+        <v>123456</v>
+      </c>
+      <c r="F20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ramon') </v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ramon'); </v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B20,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ramon', 'ramon', 'ramon@email.com', '123456'); </v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>90</v>
       </c>
       <c r="C21" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>samuel</v>
+      </c>
+      <c r="D21" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>samuel@email.com</v>
+      </c>
+      <c r="E21">
+        <v>123456</v>
+      </c>
+      <c r="F21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Samuel'); </v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H21" s="2" t="str">
+      <c r="I21" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B21,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Samuel', 'samuel', 'samuel@email.com', '123456'); </v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K21" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') , 'ssss'); </v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>91</v>
       </c>
       <c r="C22" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>tomas</v>
+      </c>
+      <c r="D22" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>tomas@email.com</v>
+      </c>
+      <c r="E22">
+        <v>123456</v>
+      </c>
+      <c r="F22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
       </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Tomas'); </v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H22" s="2" t="str">
+      <c r="I22" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B22,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Tomas', 'tomas', 'tomas@email.com', '123456'); </v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') , 'tttt'); </v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>93</v>
       </c>
       <c r="C23" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>ubaldo</v>
+      </c>
+      <c r="D23" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>ubaldo@email.com</v>
+      </c>
+      <c r="E23">
+        <v>123456</v>
+      </c>
+      <c r="F23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Ubaldo'); </v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H23" s="2" t="str">
+      <c r="I23" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B23,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ubaldo', 'ubaldo', 'ubaldo@email.com', '123456'); </v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') , 'uuuu'); </v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>92</v>
       </c>
       <c r="C24" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>veronica</v>
+      </c>
+      <c r="D24" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>veronica@email.com</v>
+      </c>
+      <c r="E24">
+        <v>123456</v>
+      </c>
+      <c r="F24" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Veronica'); </v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="2" t="str">
+      <c r="I24" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B24,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Veronica', 'veronica', 'veronica@email.com', '123456'); </v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K24" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') , 'vvvv'); </v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>94</v>
       </c>
       <c r="C25" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>wendy</v>
+      </c>
+      <c r="D25" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>wendy@email.com</v>
+      </c>
+      <c r="E25">
+        <v>123456</v>
+      </c>
+      <c r="F25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Wendy'); </v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H25" s="2" t="str">
+      <c r="I25" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B25,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Wendy', 'wendy', 'wendy@email.com', '123456'); </v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K25" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') , 'wwww'); </v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>95</v>
       </c>
       <c r="C26" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>xochil</v>
+      </c>
+      <c r="D26" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>xochil@email.com</v>
+      </c>
+      <c r="E26">
+        <v>123456</v>
+      </c>
+      <c r="F26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
       </c>
-      <c r="D26" t="s">
+      <c r="G26" t="s">
         <v>125</v>
       </c>
-      <c r="F26" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Xochil'); </v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H26" s="2" t="str">
+      <c r="I26" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B26,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Xochil', 'xochil', 'xochil@email.com', '123456'); </v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K26" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') , 'xxxx'); </v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>96</v>
       </c>
       <c r="C27" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>yolanda</v>
+      </c>
+      <c r="D27" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>yolanda@email.com</v>
+      </c>
+      <c r="E27">
+        <v>123456</v>
+      </c>
+      <c r="F27" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Yolanda'); </v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H27" s="2" t="str">
+      <c r="I27" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B27,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Yolanda', 'yolanda', 'yolanda@email.com', '123456'); </v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K27" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') , 'yyyy'); </v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>97</v>
       </c>
       <c r="C28" t="str">
+        <f>LOWER(Tabla4[[#This Row],[name]])</f>
+        <v>zoe</v>
+      </c>
+      <c r="D28" t="str">
+        <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
+        <v>zoe@email.com</v>
+      </c>
+      <c r="E28">
+        <v>123456</v>
+      </c>
+      <c r="F28" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
       </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">INSERT INTO users (NAME) VALUES ('Zoe'); </v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H28" s="2" t="str">
+      <c r="I28" s="11" t="str">
+        <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B28,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Zoe', 'zoe', 'zoe@email.com', '123456'); </v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K28" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') , 'zzzz'); </v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added valid passwords for all users (pass = 123456) Added data for Roles for user: Admin, AccountHolders and ThirdParty. #12
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="201">
   <si>
     <t>Request Type</t>
   </si>
@@ -600,6 +600,36 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK</t>
+  </si>
+  <si>
+    <t>$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>ROLE_ADMIN</t>
+  </si>
+  <si>
+    <t>ADMINS TABLE</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>ROLE_USER</t>
+  </si>
+  <si>
+    <t>ROLE_THIRDPARTY</t>
+  </si>
+  <si>
+    <t>ROLES table</t>
+  </si>
+  <si>
+    <t>Account_holders Table</t>
   </si>
 </sst>
 </file>
@@ -715,7 +745,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -757,6 +787,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
@@ -764,7 +802,20 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -776,13 +827,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -822,12 +866,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A3:G28" totalsRowShown="0">
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="11"/>
-    <tableColumn id="2" name="Request Type" dataDxfId="10"/>
+    <tableColumn id="1" name="#" dataDxfId="13"/>
+    <tableColumn id="2" name="Request Type" dataDxfId="12"/>
     <tableColumn id="5" name="Param Type"/>
-    <tableColumn id="7" name="Usuario" dataDxfId="9"/>
+    <tableColumn id="7" name="Usuario" dataDxfId="11"/>
     <tableColumn id="3" name="Endpoint"/>
-    <tableColumn id="4" name="Response Description" dataDxfId="8"/>
+    <tableColumn id="4" name="Response Description" dataDxfId="10"/>
     <tableColumn id="6" name="Requsitos o Respuesta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -841,8 +885,8 @@
     <tableColumn id="2" name="country"/>
     <tableColumn id="3" name="city"/>
     <tableColumn id="4" name="street"/>
-    <tableColumn id="5" name="house_number" dataDxfId="7"/>
-    <tableColumn id="6" name="home_unit" dataDxfId="6"/>
+    <tableColumn id="5" name="house_number" dataDxfId="9"/>
+    <tableColumn id="6" name="home_unit" dataDxfId="8"/>
     <tableColumn id="7" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -850,43 +894,45 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B19:E23" totalsRowShown="0">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B19:F23" totalsRowShown="0">
+  <tableColumns count="5">
     <tableColumn id="1" name="name"/>
-    <tableColumn id="2" name="username" dataDxfId="2">
+    <tableColumn id="2" name="username" dataDxfId="7">
       <calculatedColumnFormula>LOWER(Tabla3[[#This Row],[name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="email" dataDxfId="1">
+    <tableColumn id="3" name="email" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="password"/>
+    <tableColumn id="6" name="Rol" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:G28" totalsRowShown="0">
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:H28" totalsRowShown="0">
+  <tableColumns count="7">
     <tableColumn id="1" name="name"/>
-    <tableColumn id="5" name="username" dataDxfId="3">
+    <tableColumn id="5" name="username" dataDxfId="5">
       <calculatedColumnFormula>LOWER(Tabla4[[#This Row],[name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="email" dataDxfId="0">
+    <tableColumn id="6" name="email" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="password"/>
-    <tableColumn id="2" name="user_id" dataDxfId="5">
+    <tableColumn id="2" name="user_id" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="hashed_key"/>
+    <tableColumn id="7" name="Role" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="K2:L13" totalsRowShown="0" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="L2:M13" totalsRowShown="0" headerRowBorderDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" name="street">
       <calculatedColumnFormula>'Address &amp; Admin'!D4</calculatedColumnFormula>
@@ -1164,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1572,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:G23"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,12 +1629,21 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20" style="3" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="9" max="9" width="47" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>69</v>
       </c>
@@ -1597,8 +1652,11 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1620,8 +1678,11 @@
       <c r="G3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -1641,8 +1702,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>30</v>
       </c>
@@ -1662,8 +1726,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>30</v>
       </c>
@@ -1683,8 +1750,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -1704,8 +1774,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>30</v>
       </c>
@@ -1725,8 +1798,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -1746,8 +1822,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1767,8 +1846,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -1788,8 +1870,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>49</v>
       </c>
@@ -1809,8 +1894,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>52</v>
       </c>
@@ -1830,8 +1918,11 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1854,13 +1945,34 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J14" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J17" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -1873,8 +1985,17 @@
       <c r="E19" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>70</v>
       </c>
@@ -1886,26 +2007,42 @@
         <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
         <v>john@email.com</v>
       </c>
-      <c r="E20">
-        <v>123456</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20" s="11" t="str">
+      <c r="E20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '123456'); </v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'John') </v>
       </c>
-      <c r="L20" t="str">
-        <f>CONCATENATE("INSERT INTO admins VALUES (",J20,"); ")</f>
+      <c r="L20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" t="str">
+        <f>CONCATENATE("INSERT INTO admins VALUES (",K20,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K20," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'John')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>71</v>
       </c>
@@ -1917,26 +2054,42 @@
         <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
         <v>alfredo@email.com</v>
       </c>
-      <c r="E21">
-        <v>123456</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21" s="11" t="str">
+      <c r="E21" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '123456'); </v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') </v>
       </c>
-      <c r="L21" t="str">
-        <f t="shared" ref="L21:L23" si="0">CONCATENATE("INSERT INTO admins VALUES (",J21,"); ")</f>
+      <c r="L21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ref="M21:M23" si="0">CONCATENATE("INSERT INTO admins VALUES (",K21,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="O21" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K21," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Alfredo')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>72</v>
       </c>
@@ -1948,26 +2101,42 @@
         <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
         <v>cristian@email.com</v>
       </c>
-      <c r="E22">
-        <v>123456</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22" s="11" t="str">
+      <c r="E22" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '123456'); </v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Cristian') </v>
       </c>
-      <c r="L22" t="str">
+      <c r="L22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N22" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="O22" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K22," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Cristian')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>73</v>
       </c>
@@ -1979,23 +2148,64 @@
         <f>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</f>
         <v>raúl@email.com</v>
       </c>
-      <c r="E23">
-        <v>123456</v>
-      </c>
-      <c r="F23"/>
-      <c r="G23" s="11" t="str">
+      <c r="E23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '123456'); </v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Raúl') </v>
       </c>
-      <c r="L23" t="str">
+      <c r="L23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
+      </c>
+      <c r="N23" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="O23" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K23," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Raúl')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J24" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J25" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J26" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J27" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J28" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2150,30 +2360,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R33"/>
+  <dimension ref="B2:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U3" sqref="U3:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -2192,17 +2406,26 @@
       <c r="G2" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="H2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="U2" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>77</v>
       </c>
@@ -2214,8 +2437,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>alberto@email.com</v>
       </c>
-      <c r="E3">
-        <v>123456</v>
+      <c r="E3" t="s">
+        <v>191</v>
       </c>
       <c r="F3" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2224,37 +2447,50 @@
       <c r="G3" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="11" t="str">
+      <c r="H3" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B3,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alberto', 'alberto', 'alberto@email.com', '123456'); </v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alberto', 'alberto', 'alberto@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" t="str">
         <f>'Address &amp; Admin'!D4</f>
         <v>Numancia</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>'Address &amp; Admin'!E4</f>
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R3" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N3,", ",P3,", ","null","); ")</f>
+      <c r="R3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O3,", ",Q3,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') , '1960-02-24', (SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') , null); </v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U3" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Alberto'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>78</v>
       </c>
@@ -2266,8 +2502,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>bernardo@email.com</v>
       </c>
-      <c r="E4">
-        <v>123456</v>
+      <c r="E4" t="s">
+        <v>191</v>
       </c>
       <c r="F4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2276,37 +2512,50 @@
       <c r="G4" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="11" t="str">
+      <c r="H4" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B4,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Bernardo', 'bernardo', 'bernardo@email.com', '123456'); </v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Bernardo', 'bernardo', 'bernardo@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L4" t="str">
         <f>'Address &amp; Admin'!D5</f>
         <v>Gran Via</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>'Address &amp; Admin'!E5</f>
         <v>50</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R4" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N4,", ",P4,", ","null","); ")</f>
+      <c r="R4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S4" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O4,", ",Q4,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') , '1990-03-23', (SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') , null); </v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U4" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Bernardo'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>79</v>
       </c>
@@ -2318,8 +2567,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>carlos@email.com</v>
       </c>
-      <c r="E5">
-        <v>123456</v>
+      <c r="E5" t="s">
+        <v>191</v>
       </c>
       <c r="F5" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2328,37 +2577,50 @@
       <c r="G5" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="11" t="str">
+      <c r="H5" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B5,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Carlos', 'carlos', 'carlos@email.com', '123456'); </v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Carlos', 'carlos', 'carlos@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" t="str">
         <f>'Address &amp; Admin'!D6</f>
         <v>Napoles</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>'Address &amp; Admin'!E6</f>
         <v>12</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R5" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N5,", ",P5,", ","null","); ")</f>
+      <c r="R5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S5" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O5,", ",Q5,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') , '2000-12-12', (SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') , null); </v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U5" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Carlos'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>80</v>
       </c>
@@ -2370,8 +2632,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>daniel@email.com</v>
       </c>
-      <c r="E6">
-        <v>123456</v>
+      <c r="E6" t="s">
+        <v>191</v>
       </c>
       <c r="F6" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2380,37 +2642,50 @@
       <c r="G6" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="11" t="str">
+      <c r="H6" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B6,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Daniel', 'daniel', 'daniel@email.com', '123456'); </v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Daniel', 'daniel', 'daniel@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" t="str">
         <f>'Address &amp; Admin'!D7</f>
         <v>Dénia</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>'Address &amp; Admin'!E7</f>
         <v>54</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R6" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N6,", ",P6,", ","null","); ")</f>
+      <c r="R6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S6" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O6,", ",Q6,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') , '1998-09-20', (SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') , null); </v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U6" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Daniel'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>81</v>
       </c>
@@ -2422,8 +2697,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ernesto@email.com</v>
       </c>
-      <c r="E7">
-        <v>123456</v>
+      <c r="E7" t="s">
+        <v>191</v>
       </c>
       <c r="F7" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2432,37 +2707,50 @@
       <c r="G7" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="11" t="str">
+      <c r="H7" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B7,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ernesto', 'ernesto', 'ernesto@email.com', '123456'); </v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ernesto', 'ernesto', 'ernesto@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L7" t="str">
         <f>'Address &amp; Admin'!D8</f>
         <v>San Blas</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>'Address &amp; Admin'!E8</f>
         <v>26</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R7" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N7,", ",P7,", ","null","); ")</f>
+      <c r="R7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S7" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O7,", ",Q7,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') , '1997-12-30', (SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') , null); </v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U7" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ernesto'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>82</v>
       </c>
@@ -2474,8 +2762,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>fernando@email.com</v>
       </c>
-      <c r="E8">
-        <v>123456</v>
+      <c r="E8" t="s">
+        <v>191</v>
       </c>
       <c r="F8" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2484,37 +2772,50 @@
       <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="H8" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B8,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Fernando', 'fernando', 'fernando@email.com', '123456'); </v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Fernando', 'fernando', 'fernando@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L8" t="str">
         <f>'Address &amp; Admin'!D9</f>
         <v>Rivolí</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>'Address &amp; Admin'!E9</f>
         <v>11</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R8" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N8,", ",P8,", ","null","); ")</f>
+      <c r="R8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S8" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O8,", ",Q8,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') , '1992-06-10', (SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') , null); </v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U8" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Fernando'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>100</v>
       </c>
@@ -2526,8 +2827,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>gladys@email.com</v>
       </c>
-      <c r="E9">
-        <v>123456</v>
+      <c r="E9" t="s">
+        <v>191</v>
       </c>
       <c r="F9" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2536,37 +2837,50 @@
       <c r="G9" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="11" t="str">
+      <c r="H9" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B9,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Gladys', 'gladys', 'gladys@email.com', '123456'); </v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Gladys', 'gladys', 'gladys@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" t="str">
         <f>'Address &amp; Admin'!D10</f>
         <v>Oberweg</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>'Address &amp; Admin'!E10</f>
         <v>69</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R9" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N9,", ",P9,", ","null","); ")</f>
+      <c r="R9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S9" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O9,", ",Q9,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') , '2001-10-05', (SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') , null); </v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U9" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Gladys'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>83</v>
       </c>
@@ -2578,8 +2892,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>hernan@email.com</v>
       </c>
-      <c r="E10">
-        <v>123456</v>
+      <c r="E10" t="s">
+        <v>191</v>
       </c>
       <c r="F10" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2588,37 +2902,50 @@
       <c r="G10" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="11" t="str">
+      <c r="H10" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B10,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Hernan', 'hernan', 'hernan@email.com', '123456'); </v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Hernan', 'hernan', 'hernan@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10" t="str">
         <f>'Address &amp; Admin'!D11</f>
         <v>Av El Dorado</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f>'Address &amp; Admin'!E11</f>
         <v>89</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R10" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N10,", ",P10,", ","null","); ")</f>
+      <c r="R10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S10" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O10,", ",Q10,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') , '1997-04-05', (SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') , null); </v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U10" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Hernan'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>84</v>
       </c>
@@ -2630,8 +2957,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ivan@email.com</v>
       </c>
-      <c r="E11">
-        <v>123456</v>
+      <c r="E11" t="s">
+        <v>191</v>
       </c>
       <c r="F11" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2640,37 +2967,50 @@
       <c r="G11" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="11" t="str">
+      <c r="H11" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B11,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ivan', 'ivan', 'ivan@email.com', '123456'); </v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ivan', 'ivan', 'ivan@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L11" t="str">
         <f>'Address &amp; Admin'!D12</f>
         <v>Jirón Callao</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f>'Address &amp; Admin'!E12</f>
         <v>24</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R11" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N11,", ",P11,", ","null","); ")</f>
+      <c r="R11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S11" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O11,", ",Q11,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') , '1975-09-13', (SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') , null); </v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U11" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ivan'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>85</v>
       </c>
@@ -2682,8 +3022,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>jose@email.com</v>
       </c>
-      <c r="E12">
-        <v>123456</v>
+      <c r="E12" t="s">
+        <v>191</v>
       </c>
       <c r="F12" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2692,37 +3032,50 @@
       <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="11" t="str">
+      <c r="H12" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B12,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Jose', 'jose', 'jose@email.com', '123456'); </v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K12" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Jose', 'jose', 'jose@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" t="str">
         <f>'Address &amp; Admin'!D13</f>
         <v>Av 9 de Julio</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>'Address &amp; Admin'!E13</f>
         <v>48</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q12" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R12" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N12,", ",P12,", ","null","); ")</f>
+      <c r="R12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S12" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O12,", ",Q12,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Jose') , '1984-09-28', (SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') , null); </v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U12" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Jose'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>86</v>
       </c>
@@ -2734,8 +3087,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>kevin@email.com</v>
       </c>
-      <c r="E13">
-        <v>123456</v>
+      <c r="E13" t="s">
+        <v>191</v>
       </c>
       <c r="F13" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2744,37 +3097,50 @@
       <c r="G13" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="11" t="str">
+      <c r="H13" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J13" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B13,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Kevin', 'kevin', 'kevin@email.com', '123456'); </v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K13" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Kevin', 'kevin', 'kevin@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" t="str">
         <f>'Address &amp; Admin'!D14</f>
         <v>Paseo de Montejo</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f>'Address &amp; Admin'!E14</f>
         <v>33</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="P13" t="str">
+      <c r="Q13" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R13" t="str">
-        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",N13,", ",P13,", ","null","); ")</f>
+      <c r="R13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="S13" t="str">
+        <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O13,", ",Q13,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') , '1982-12-02', (SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') , null); </v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U13" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Kevin'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>99</v>
       </c>
@@ -2786,8 +3152,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>liliana@email.com</v>
       </c>
-      <c r="E14">
-        <v>123456</v>
+      <c r="E14" t="s">
+        <v>191</v>
       </c>
       <c r="F14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2796,18 +3162,25 @@
       <c r="G14" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="11" t="str">
+      <c r="H14" s="21"/>
+      <c r="I14" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B14,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Liliana', 'liliana', 'liliana@email.com', '123456'); </v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Liliana', 'liliana', 'liliana@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>98</v>
       </c>
@@ -2819,8 +3192,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>maria@email.com</v>
       </c>
-      <c r="E15">
-        <v>123456</v>
+      <c r="E15" t="s">
+        <v>191</v>
       </c>
       <c r="F15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2829,18 +3202,25 @@
       <c r="G15" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="11" t="str">
+      <c r="H15" s="21"/>
+      <c r="I15" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B15,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Maria', 'maria', 'maria@email.com', '123456'); </v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Maria', 'maria', 'maria@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>128</v>
       </c>
@@ -2852,8 +3232,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>nancy@email.com</v>
       </c>
-      <c r="E16">
-        <v>123456</v>
+      <c r="E16" t="s">
+        <v>191</v>
       </c>
       <c r="F16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2862,18 +3242,25 @@
       <c r="G16" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="11" t="str">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J16" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B16,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Nancy', 'nancy', 'nancy@email.com', '123456'); </v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Nancy', 'nancy', 'nancy@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>87</v>
       </c>
@@ -2885,8 +3272,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>orlando@email.com</v>
       </c>
-      <c r="E17">
-        <v>123456</v>
+      <c r="E17" t="s">
+        <v>191</v>
       </c>
       <c r="F17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2895,18 +3282,25 @@
       <c r="G17" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="11" t="str">
+      <c r="H17" s="21"/>
+      <c r="I17" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J17" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B17,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Orlando', 'orlando', 'orlando@email.com', '123456'); </v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Orlando', 'orlando', 'orlando@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>88</v>
       </c>
@@ -2918,8 +3312,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>pedro@email.com</v>
       </c>
-      <c r="E18">
-        <v>123456</v>
+      <c r="E18" t="s">
+        <v>191</v>
       </c>
       <c r="F18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2928,18 +3322,25 @@
       <c r="G18" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="11" t="str">
+      <c r="H18" s="21"/>
+      <c r="I18" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B18,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Pedro', 'pedro', 'pedro@email.com', '123456'); </v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Pedro', 'pedro', 'pedro@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>101</v>
       </c>
@@ -2951,8 +3352,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>quentin@email.com</v>
       </c>
-      <c r="E19">
-        <v>123456</v>
+      <c r="E19" t="s">
+        <v>191</v>
       </c>
       <c r="F19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2961,18 +3362,25 @@
       <c r="G19" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="11" t="str">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B19,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Quentin', 'quentin', 'quentin@email.com', '123456'); </v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Quentin', 'quentin', 'quentin@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>89</v>
       </c>
@@ -2984,8 +3392,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ramon@email.com</v>
       </c>
-      <c r="E20">
-        <v>123456</v>
+      <c r="E20" t="s">
+        <v>191</v>
       </c>
       <c r="F20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2994,18 +3402,28 @@
       <c r="G20" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="11" t="str">
+      <c r="H20" s="21"/>
+      <c r="I20" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B20,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ramon', 'ramon', 'ramon@email.com', '123456'); </v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ramon', 'ramon', 'ramon@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>90</v>
       </c>
@@ -3017,8 +3435,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>samuel@email.com</v>
       </c>
-      <c r="E21">
-        <v>123456</v>
+      <c r="E21" t="s">
+        <v>191</v>
       </c>
       <c r="F21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3027,19 +3445,32 @@
       <c r="G21" t="s">
         <v>120</v>
       </c>
-      <c r="I21" s="11" t="str">
+      <c r="H21" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B21,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Samuel', 'samuel', 'samuel@email.com', '123456'); </v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K21" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Samuel', 'samuel', 'samuel@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') , 'ssss'); </v>
       </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O21" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Samuel'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>91</v>
       </c>
@@ -3051,8 +3482,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>tomas@email.com</v>
       </c>
-      <c r="E22">
-        <v>123456</v>
+      <c r="E22" t="s">
+        <v>191</v>
       </c>
       <c r="F22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3061,19 +3492,32 @@
       <c r="G22" t="s">
         <v>121</v>
       </c>
-      <c r="I22" s="11" t="str">
+      <c r="H22" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B22,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Tomas', 'tomas', 'tomas@email.com', '123456'); </v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K22" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Tomas', 'tomas', 'tomas@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') , 'tttt'); </v>
       </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O22" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Tomas'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>93</v>
       </c>
@@ -3085,8 +3529,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ubaldo@email.com</v>
       </c>
-      <c r="E23">
-        <v>123456</v>
+      <c r="E23" t="s">
+        <v>191</v>
       </c>
       <c r="F23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3095,19 +3539,32 @@
       <c r="G23" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="11" t="str">
+      <c r="H23" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B23,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ubaldo', 'ubaldo', 'ubaldo@email.com', '123456'); </v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ubaldo', 'ubaldo', 'ubaldo@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L23" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') , 'uuuu'); </v>
       </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O23" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ubaldo'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>92</v>
       </c>
@@ -3119,8 +3576,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>veronica@email.com</v>
       </c>
-      <c r="E24">
-        <v>123456</v>
+      <c r="E24" t="s">
+        <v>191</v>
       </c>
       <c r="F24" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3129,19 +3586,32 @@
       <c r="G24" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="11" t="str">
+      <c r="H24" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B24,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Veronica', 'veronica', 'veronica@email.com', '123456'); </v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K24" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Veronica', 'veronica', 'veronica@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L24" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') , 'vvvv'); </v>
       </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O24" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Veronica'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>94</v>
       </c>
@@ -3153,8 +3623,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>wendy@email.com</v>
       </c>
-      <c r="E25">
-        <v>123456</v>
+      <c r="E25" t="s">
+        <v>191</v>
       </c>
       <c r="F25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3163,19 +3633,32 @@
       <c r="G25" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="11" t="str">
+      <c r="H25" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B25,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Wendy', 'wendy', 'wendy@email.com', '123456'); </v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K25" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Wendy', 'wendy', 'wendy@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') , 'wwww'); </v>
       </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O25" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Wendy'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>95</v>
       </c>
@@ -3187,8 +3670,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>xochil@email.com</v>
       </c>
-      <c r="E26">
-        <v>123456</v>
+      <c r="E26" t="s">
+        <v>191</v>
       </c>
       <c r="F26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3197,19 +3680,32 @@
       <c r="G26" t="s">
         <v>125</v>
       </c>
-      <c r="I26" s="11" t="str">
+      <c r="H26" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B26,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Xochil', 'xochil', 'xochil@email.com', '123456'); </v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K26" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Xochil', 'xochil', 'xochil@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L26" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') , 'xxxx'); </v>
       </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O26" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Xochil'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>96</v>
       </c>
@@ -3221,8 +3717,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>yolanda@email.com</v>
       </c>
-      <c r="E27">
-        <v>123456</v>
+      <c r="E27" t="s">
+        <v>191</v>
       </c>
       <c r="F27" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3231,19 +3727,32 @@
       <c r="G27" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="11" t="str">
+      <c r="H27" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B27,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Yolanda', 'yolanda', 'yolanda@email.com', '123456'); </v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K27" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Yolanda', 'yolanda', 'yolanda@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') , 'yyyy'); </v>
       </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O27" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Yolanda'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>97</v>
       </c>
@@ -3255,8 +3764,8 @@
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>zoe@email.com</v>
       </c>
-      <c r="E28">
-        <v>123456</v>
+      <c r="E28" t="s">
+        <v>191</v>
       </c>
       <c r="F28" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3265,24 +3774,42 @@
       <c r="G28" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="11" t="str">
+      <c r="H28" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B28,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
-        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Zoe', 'zoe', 'zoe@email.com', '123456'); </v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K28" s="2" t="str">
+        <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Zoe', 'zoe', 'zoe@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L28" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') , 'zzzz'); </v>
       </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O28" t="str">
+        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Zoe'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
Fixed inserts in 'users_roles' table and changed column name 'id' -> 'role_id' in 'roles' table. #12
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
@@ -781,12 +781,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -794,6 +788,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -803,12 +803,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thick">
@@ -824,6 +818,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -904,7 +904,7 @@
       <calculatedColumnFormula>CONCATENATE(Tabla3[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="password"/>
-    <tableColumn id="6" name="Rol" dataDxfId="1"/>
+    <tableColumn id="6" name="Rol" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -914,25 +914,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B2:H28" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="name"/>
-    <tableColumn id="5" name="username" dataDxfId="5">
+    <tableColumn id="5" name="username" dataDxfId="4">
       <calculatedColumnFormula>LOWER(Tabla4[[#This Row],[name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="email" dataDxfId="4">
+    <tableColumn id="6" name="email" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="password"/>
-    <tableColumn id="2" name="user_id" dataDxfId="3">
+    <tableColumn id="2" name="user_id" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="hashed_key"/>
-    <tableColumn id="7" name="Role" dataDxfId="0"/>
+    <tableColumn id="7" name="Role" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="L2:M13" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="L2:M13" totalsRowShown="0" headerRowBorderDxfId="0">
   <tableColumns count="2">
     <tableColumn id="1" name="street">
       <calculatedColumnFormula>'Address &amp; Admin'!D4</calculatedColumnFormula>
@@ -1210,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1226,13 +1226,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1639,20 +1639,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="J2" s="19" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="J2" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
       <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1798,7 +1798,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1918,7 +1918,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1945,22 +1945,22 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1968,7 +1968,7 @@
       <c r="B18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1988,10 +1988,10 @@
       <c r="F19" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="M19" s="20" t="s">
+      <c r="J19" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="18" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="17" t="s">
         <v>141</v>
       </c>
       <c r="K20" t="str">
@@ -2034,12 +2034,12 @@
         <f>CONCATENATE("INSERT INTO admins VALUES (",K20,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="17" t="s">
         <v>141</v>
       </c>
       <c r="O20" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K20," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'John')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K20," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'John')  ), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -2067,7 +2067,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="17" t="s">
         <v>141</v>
       </c>
       <c r="K21" t="str">
@@ -2081,12 +2081,12 @@
         <f t="shared" ref="M21:M23" si="0">CONCATENATE("INSERT INTO admins VALUES (",K21,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="17" t="s">
         <v>141</v>
       </c>
       <c r="O21" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K21," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Alfredo')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K21," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Alfredo')  ), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="17" t="s">
         <v>141</v>
       </c>
       <c r="K22" t="str">
@@ -2128,12 +2128,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="17" t="s">
         <v>141</v>
       </c>
       <c r="O22" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K22," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Cristian')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K22," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Cristian')  ), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2161,7 +2161,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="17" t="s">
         <v>141</v>
       </c>
       <c r="K23" t="str">
@@ -2175,36 +2175,36 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="17" t="s">
         <v>141</v>
       </c>
       <c r="O23" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES(","( ",K23," ), ( ","SELECT ID FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Raúl')  ), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K23," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES(( (SELECT user_id FROM users WHERE NAME LIKE 'Raúl')  ), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_ADMIN' ) ); </v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2362,8 +2362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:U13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U3:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,10 +2418,10 @@
       <c r="O2" t="s">
         <v>140</v>
       </c>
-      <c r="S2" s="23" t="s">
+      <c r="S2" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="22" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2447,10 +2447,10 @@
       <c r="G3" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J3" s="11" t="str">
@@ -2486,8 +2486,8 @@
         <v>141</v>
       </c>
       <c r="U3" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Alberto'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Alberto'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
@@ -2512,10 +2512,10 @@
       <c r="G4" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J4" s="11" t="str">
@@ -2551,8 +2551,8 @@
         <v>141</v>
       </c>
       <c r="U4" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Bernardo'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Bernardo'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
@@ -2577,10 +2577,10 @@
       <c r="G5" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J5" s="11" t="str">
@@ -2616,8 +2616,8 @@
         <v>141</v>
       </c>
       <c r="U5" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Carlos'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Carlos'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -2642,10 +2642,10 @@
       <c r="G6" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J6" s="11" t="str">
@@ -2681,8 +2681,8 @@
         <v>141</v>
       </c>
       <c r="U6" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Daniel'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Daniel'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
@@ -2707,10 +2707,10 @@
       <c r="G7" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J7" s="11" t="str">
@@ -2746,8 +2746,8 @@
         <v>141</v>
       </c>
       <c r="U7" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ernesto'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ernesto'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
@@ -2772,10 +2772,10 @@
       <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J8" s="11" t="str">
@@ -2811,8 +2811,8 @@
         <v>141</v>
       </c>
       <c r="U8" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Fernando'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Fernando'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
@@ -2837,10 +2837,10 @@
       <c r="G9" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J9" s="11" t="str">
@@ -2876,8 +2876,8 @@
         <v>141</v>
       </c>
       <c r="U9" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Gladys'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Gladys'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
@@ -2902,10 +2902,10 @@
       <c r="G10" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J10" s="11" t="str">
@@ -2941,8 +2941,8 @@
         <v>141</v>
       </c>
       <c r="U10" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Hernan'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Hernan'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
@@ -2967,10 +2967,10 @@
       <c r="G11" t="s">
         <v>110</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J11" s="11" t="str">
@@ -3006,8 +3006,8 @@
         <v>141</v>
       </c>
       <c r="U11" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ivan'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ivan'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
@@ -3032,10 +3032,10 @@
       <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J12" s="11" t="str">
@@ -3071,8 +3071,8 @@
         <v>141</v>
       </c>
       <c r="U12" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Jose'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Jose'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
@@ -3097,10 +3097,10 @@
       <c r="G13" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J13" s="11" t="str">
@@ -3136,8 +3136,8 @@
         <v>141</v>
       </c>
       <c r="U13" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Kevin'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Kevin'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_USER') ); </v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
@@ -3162,8 +3162,8 @@
       <c r="G14" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22" t="s">
+      <c r="H14" s="19"/>
+      <c r="I14" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J14" s="11" t="str">
@@ -3202,8 +3202,8 @@
       <c r="G15" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J15" s="11" t="str">
@@ -3242,8 +3242,8 @@
       <c r="G16" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22" t="s">
+      <c r="H16" s="19"/>
+      <c r="I16" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J16" s="11" t="str">
@@ -3282,8 +3282,8 @@
       <c r="G17" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22" t="s">
+      <c r="H17" s="19"/>
+      <c r="I17" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J17" s="11" t="str">
@@ -3322,8 +3322,8 @@
       <c r="G18" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22" t="s">
+      <c r="H18" s="19"/>
+      <c r="I18" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J18" s="11" t="str">
@@ -3362,8 +3362,8 @@
       <c r="G19" t="s">
         <v>118</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="19"/>
+      <c r="I19" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J19" s="11" t="str">
@@ -3402,8 +3402,8 @@
       <c r="G20" t="s">
         <v>119</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22" t="s">
+      <c r="H20" s="19"/>
+      <c r="I20" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J20" s="11" t="str">
@@ -3413,7 +3413,7 @@
       <c r="K20" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="O20" s="24" t="s">
+      <c r="O20" s="22" t="s">
         <v>199</v>
       </c>
       <c r="R20" s="2" t="s">
@@ -3445,10 +3445,10 @@
       <c r="G21" t="s">
         <v>120</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J21" s="11" t="str">
@@ -3466,8 +3466,8 @@
         <v>141</v>
       </c>
       <c r="O21" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Samuel'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Samuel'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
@@ -3492,10 +3492,10 @@
       <c r="G22" t="s">
         <v>121</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J22" s="11" t="str">
@@ -3513,8 +3513,8 @@
         <v>141</v>
       </c>
       <c r="O22" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Tomas'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Tomas'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
@@ -3539,10 +3539,10 @@
       <c r="G23" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J23" s="11" t="str">
@@ -3560,8 +3560,8 @@
         <v>141</v>
       </c>
       <c r="O23" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ubaldo'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Ubaldo'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
@@ -3586,10 +3586,10 @@
       <c r="G24" t="s">
         <v>123</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J24" s="11" t="str">
@@ -3607,8 +3607,8 @@
         <v>141</v>
       </c>
       <c r="O24" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Veronica'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Veronica'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -3633,10 +3633,10 @@
       <c r="G25" t="s">
         <v>124</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J25" s="11" t="str">
@@ -3654,8 +3654,8 @@
         <v>141</v>
       </c>
       <c r="O25" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Wendy'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Wendy'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -3680,10 +3680,10 @@
       <c r="G26" t="s">
         <v>125</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J26" s="11" t="str">
@@ -3701,8 +3701,8 @@
         <v>141</v>
       </c>
       <c r="O26" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Xochil'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Xochil'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
@@ -3727,10 +3727,10 @@
       <c r="G27" t="s">
         <v>126</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J27" s="11" t="str">
@@ -3748,8 +3748,8 @@
         <v>141</v>
       </c>
       <c r="O27" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Yolanda'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Yolanda'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -3774,10 +3774,10 @@
       <c r="G28" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="20" t="s">
         <v>141</v>
       </c>
       <c r="J28" s="11" t="str">
@@ -3795,8 +3795,8 @@
         <v>141</v>
       </c>
       <c r="O28" t="str">
-        <f>CONCATENATE("INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT ID FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
-        <v xml:space="preserve">INSERT INTO user_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Zoe'), ( SELECT ID FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
+        <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
+        <v xml:space="preserve">INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE 'Zoe'), ( SELECT role_id FROM roles WHERE role_name LIKE 'ROLE_THIRDPARTY') ); </v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated info about implementing security and how to update the existing some endpoints. #4
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26955" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="EndPoints" sheetId="1" r:id="rId1"/>
@@ -461,9 +461,6 @@
     <t>crear un ThirdParty user</t>
   </si>
   <si>
-    <t>/admins</t>
-  </si>
-  <si>
     <t>/admins/accountholders</t>
   </si>
   <si>
@@ -630,6 +627,9 @@
   </si>
   <si>
     <t>Account_holders Table</t>
+  </si>
+  <si>
+    <t>/admins/welcome</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
@@ -1279,13 +1279,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
         <v>178</v>
       </c>
-      <c r="F5" t="s">
-        <v>179</v>
-      </c>
       <c r="G5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1293,56 +1293,56 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F6" t="s">
         <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" t="s">
         <v>149</v>
-      </c>
-      <c r="G7" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10"/>
       <c r="E10" s="2"/>
       <c r="F10" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" t="s">
         <v>155</v>
-      </c>
-      <c r="G10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,13 +1357,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,14 +1376,14 @@
       <c r="D13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>172</v>
+      <c r="E13" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,8 +1396,8 @@
       <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>146</v>
+      <c r="E14" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>15</v>
@@ -1413,8 +1413,8 @@
       <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>147</v>
+      <c r="E15" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
@@ -1428,13 +1428,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>19</v>
@@ -1459,13 +1459,13 @@
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1475,14 +1475,14 @@
       <c r="D19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>180</v>
+      <c r="E19" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -1492,14 +1492,14 @@
       <c r="D20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>181</v>
+      <c r="E20" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1510,10 +1510,10 @@
         <v>11</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
@@ -1548,7 +1548,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>19</v>
@@ -1562,13 +1562,13 @@
         <v>17</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="G26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1578,19 +1578,19 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" t="s">
         <v>168</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G28" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1977,22 +1977,22 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
         <v>188</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>189</v>
       </c>
-      <c r="E19" t="s">
-        <v>190</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>141</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -2008,10 +2008,10 @@
         <v>john@email.com</v>
       </c>
       <c r="E20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>141</v>
@@ -2055,10 +2055,10 @@
         <v>alfredo@email.com</v>
       </c>
       <c r="E21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>141</v>
@@ -2102,10 +2102,10 @@
         <v>cristian@email.com</v>
       </c>
       <c r="E22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>141</v>
@@ -2149,10 +2149,10 @@
         <v>raúl@email.com</v>
       </c>
       <c r="E23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>141</v>
@@ -2362,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U13" sqref="U3:U13"/>
     </sheetView>
   </sheetViews>
@@ -2392,13 +2392,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
         <v>188</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>189</v>
-      </c>
-      <c r="E2" t="s">
-        <v>190</v>
       </c>
       <c r="F2" t="s">
         <v>75</v>
@@ -2407,7 +2407,7 @@
         <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>26</v>
@@ -2419,10 +2419,10 @@
         <v>140</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>alberto@email.com</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F3" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2448,7 +2448,7 @@
         <v>102</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>141</v>
@@ -2503,7 +2503,7 @@
         <v>bernardo@email.com</v>
       </c>
       <c r="E4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2513,7 +2513,7 @@
         <v>103</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>141</v>
@@ -2568,7 +2568,7 @@
         <v>carlos@email.com</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F5" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2578,7 +2578,7 @@
         <v>104</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>141</v>
@@ -2633,7 +2633,7 @@
         <v>daniel@email.com</v>
       </c>
       <c r="E6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F6" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2643,7 +2643,7 @@
         <v>105</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>141</v>
@@ -2698,7 +2698,7 @@
         <v>ernesto@email.com</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2708,7 +2708,7 @@
         <v>106</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>141</v>
@@ -2763,7 +2763,7 @@
         <v>fernando@email.com</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2773,7 +2773,7 @@
         <v>107</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>141</v>
@@ -2828,7 +2828,7 @@
         <v>gladys@email.com</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F9" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2838,7 +2838,7 @@
         <v>108</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>141</v>
@@ -2893,7 +2893,7 @@
         <v>hernan@email.com</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F10" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2903,7 +2903,7 @@
         <v>109</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I10" s="20" t="s">
         <v>141</v>
@@ -2958,7 +2958,7 @@
         <v>ivan@email.com</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F11" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2968,7 +2968,7 @@
         <v>110</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I11" s="20" t="s">
         <v>141</v>
@@ -3023,7 +3023,7 @@
         <v>jose@email.com</v>
       </c>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3033,7 +3033,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>141</v>
@@ -3088,7 +3088,7 @@
         <v>kevin@email.com</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3098,7 +3098,7 @@
         <v>112</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>141</v>
@@ -3153,7 +3153,7 @@
         <v>liliana@email.com</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3193,7 +3193,7 @@
         <v>maria@email.com</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3233,7 +3233,7 @@
         <v>nancy@email.com</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3273,7 +3273,7 @@
         <v>orlando@email.com</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3313,7 +3313,7 @@
         <v>pedro@email.com</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3353,7 +3353,7 @@
         <v>quentin@email.com</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3393,7 +3393,7 @@
         <v>ramon@email.com</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3414,7 +3414,7 @@
         <v>141</v>
       </c>
       <c r="O20" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>141</v>
@@ -3436,7 +3436,7 @@
         <v>samuel@email.com</v>
       </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3446,7 +3446,7 @@
         <v>120</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>141</v>
@@ -3483,7 +3483,7 @@
         <v>tomas@email.com</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3493,7 +3493,7 @@
         <v>121</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>141</v>
@@ -3530,7 +3530,7 @@
         <v>ubaldo@email.com</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3540,7 +3540,7 @@
         <v>122</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>141</v>
@@ -3577,7 +3577,7 @@
         <v>veronica@email.com</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F24" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3587,7 +3587,7 @@
         <v>123</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>141</v>
@@ -3624,7 +3624,7 @@
         <v>wendy@email.com</v>
       </c>
       <c r="E25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3634,7 +3634,7 @@
         <v>124</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>141</v>
@@ -3671,7 +3671,7 @@
         <v>xochil@email.com</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3681,7 +3681,7 @@
         <v>125</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>141</v>
@@ -3718,7 +3718,7 @@
         <v>yolanda@email.com</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F27" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3728,7 +3728,7 @@
         <v>126</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I27" s="20" t="s">
         <v>141</v>
@@ -3765,7 +3765,7 @@
         <v>zoe@email.com</v>
       </c>
       <c r="E28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F28" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -3775,7 +3775,7 @@
         <v>127</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>141</v>
@@ -3801,22 +3801,22 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update about the project progress showing the new defined ednpoints. #1
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -1211,7 +1211,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1376,7 @@
       <c r="D13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="14" t="s">
         <v>171</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1396,7 +1396,7 @@
       <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="14" t="s">
         <v>145</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1413,7 +1413,7 @@
       <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="14" t="s">
         <v>146</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1475,7 +1475,7 @@
       <c r="D19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="14" t="s">
         <v>179</v>
       </c>
       <c r="F19" s="1" t="s">

</xml_diff>

<commit_message>
Update for external files in the project. #1
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="239">
   <si>
     <t>Request Type</t>
   </si>
@@ -83,9 +83,6 @@
     <t>AccountHolder</t>
   </si>
   <si>
-    <t>Muestra todas sus cuentas</t>
-  </si>
-  <si>
     <t>Muestra el detalle de una especifica cuenta.</t>
   </si>
   <si>
@@ -512,9 +509,6 @@
     <t>IBAN, anterior saldo, nuevo saldo</t>
   </si>
   <si>
-    <t>/accountholder/{id}</t>
-  </si>
-  <si>
     <t>/accountholder/{id}/{IBAN}</t>
   </si>
   <si>
@@ -744,6 +738,12 @@
   </si>
   <si>
     <t>Accounts table</t>
+  </si>
+  <si>
+    <t>/accountholder/welcome</t>
+  </si>
+  <si>
+    <t>Muestra las cuentas del usuario</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
@@ -1454,76 +1454,76 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" t="s">
         <v>148</v>
-      </c>
-      <c r="G7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10"/>
       <c r="E10" s="2"/>
       <c r="F10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" t="s">
         <v>154</v>
-      </c>
-      <c r="G10" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1538,13 +1538,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1558,13 +1558,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>15</v>
@@ -1595,7 +1595,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
@@ -1609,13 +1609,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1626,75 +1626,75 @@
         <v>11</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1703,22 +1703,24 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="2"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>161</v>
+      <c r="E24" s="14" t="s">
+        <v>237</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1729,27 +1731,27 @@
         <v>17</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1759,19 +1761,19 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="F28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" t="s">
         <v>166</v>
-      </c>
-      <c r="G28" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1831,42 +1833,42 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
         <v>186</v>
       </c>
-      <c r="D2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" t="s">
-        <v>188</v>
-      </c>
       <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
       <c r="H2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="O2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -1877,27 +1879,27 @@
         <v>alberto@email.com</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F3" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J3" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B3,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alberto', 'alberto', 'alberto@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L3" t="str">
         <f>'Address &amp; Admin'!D4</f>
@@ -1908,21 +1910,21 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q3" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') </v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S3" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O3,", ",Q3,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') , '1960-02-24', (SELECT address_id FROM addresses WHERE street LIKE 'Numancia' AND house_number LIKE '23') , null); </v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U3" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -1931,7 +1933,7 @@
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -1942,27 +1944,27 @@
         <v>bernardo@email.com</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F4" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J4" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B4,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Bernardo', 'bernardo', 'bernardo@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L4" t="str">
         <f>'Address &amp; Admin'!D5</f>
@@ -1973,21 +1975,21 @@
         <v>50</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q4" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') </v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S4" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O4,", ",Q4,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') , '1990-03-23', (SELECT address_id FROM addresses WHERE street LIKE 'Gran Via' AND house_number LIKE '50') , null); </v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U4" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -1996,7 +1998,7 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2007,27 +2009,27 @@
         <v>carlos@email.com</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F5" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J5" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B5,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Carlos', 'carlos', 'carlos@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L5" t="str">
         <f>'Address &amp; Admin'!D6</f>
@@ -2038,21 +2040,21 @@
         <v>12</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q5" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') </v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S5" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O5,", ",Q5,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') , '2000-12-12', (SELECT address_id FROM addresses WHERE street LIKE 'Napoles' AND house_number LIKE '12') , null); </v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U5" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2061,7 +2063,7 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2072,27 +2074,27 @@
         <v>daniel@email.com</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F6" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J6" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B6,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Daniel', 'daniel', 'daniel@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L6" t="str">
         <f>'Address &amp; Admin'!D7</f>
@@ -2103,21 +2105,21 @@
         <v>54</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q6" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') </v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S6" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O6,", ",Q6,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') , '1998-09-20', (SELECT address_id FROM addresses WHERE street LIKE 'Dénia' AND house_number LIKE '54') , null); </v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U6" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2126,7 +2128,7 @@
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2137,27 +2139,27 @@
         <v>ernesto@email.com</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F7" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J7" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B7,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ernesto', 'ernesto', 'ernesto@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L7" t="str">
         <f>'Address &amp; Admin'!D8</f>
@@ -2168,21 +2170,21 @@
         <v>26</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q7" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') </v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S7" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O7,", ",Q7,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') , '1997-12-30', (SELECT address_id FROM addresses WHERE street LIKE 'San Blas' AND house_number LIKE '26') , null); </v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U7" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2191,7 +2193,7 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2202,27 +2204,27 @@
         <v>fernando@email.com</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F8" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J8" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B8,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Fernando', 'fernando', 'fernando@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L8" t="str">
         <f>'Address &amp; Admin'!D9</f>
@@ -2233,21 +2235,21 @@
         <v>11</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q8" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') </v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S8" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O8,", ",Q8,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') , '1992-06-10', (SELECT address_id FROM addresses WHERE street LIKE 'Rivolí' AND house_number LIKE '11') , null); </v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U8" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2256,7 +2258,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2267,27 +2269,27 @@
         <v>gladys@email.com</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F9" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J9" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B9,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Gladys', 'gladys', 'gladys@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L9" t="str">
         <f>'Address &amp; Admin'!D10</f>
@@ -2298,21 +2300,21 @@
         <v>69</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q9" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') </v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S9" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O9,", ",Q9,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') , '2001-10-05', (SELECT address_id FROM addresses WHERE street LIKE 'Oberweg' AND house_number LIKE '69') , null); </v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U9" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2321,7 +2323,7 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2332,27 +2334,27 @@
         <v>hernan@email.com</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F10" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J10" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B10,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Hernan', 'hernan', 'hernan@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L10" t="str">
         <f>'Address &amp; Admin'!D11</f>
@@ -2363,21 +2365,21 @@
         <v>89</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q10" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') </v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S10" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O10,", ",Q10,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') , '1997-04-05', (SELECT address_id FROM addresses WHERE street LIKE 'Av El Dorado' AND house_number LIKE '89') , null); </v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U10" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2386,7 +2388,7 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2397,27 +2399,27 @@
         <v>ivan@email.com</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F11" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J11" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B11,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ivan', 'ivan', 'ivan@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L11" t="str">
         <f>'Address &amp; Admin'!D12</f>
@@ -2428,21 +2430,21 @@
         <v>24</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q11" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') </v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S11" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O11,", ",Q11,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') , '1975-09-13', (SELECT address_id FROM addresses WHERE street LIKE 'Jirón Callao' AND house_number LIKE '24') , null); </v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U11" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2451,7 +2453,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2462,27 +2464,27 @@
         <v>jose@email.com</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F12" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J12" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B12,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Jose', 'jose', 'jose@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L12" t="str">
         <f>'Address &amp; Admin'!D13</f>
@@ -2493,21 +2495,21 @@
         <v>48</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q12" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') </v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S12" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O12,", ",Q12,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Jose') , '1984-09-28', (SELECT address_id FROM addresses WHERE street LIKE 'Av 9 de Julio' AND house_number LIKE '48') , null); </v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U12" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2516,7 +2518,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2527,27 +2529,27 @@
         <v>kevin@email.com</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F13" s="17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J13" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B13,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Kevin', 'kevin', 'kevin@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L13" t="str">
         <f>'Address &amp; Admin'!D14</f>
@@ -2558,21 +2560,21 @@
         <v>33</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q13" t="str">
         <f>CONCATENATE("(SELECT address_id FROM addresses WHERE street LIKE '",Tabla5[[#This Row],[street]],"' AND house_number LIKE '",Tabla5[[#This Row],[house_number]],"') ")</f>
         <v xml:space="preserve">(SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') </v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S13" t="str">
         <f>CONCATENATE("INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES (",Tabla4[[#This Row],[user_id]],", '",O13,", ",Q13,", ","null","); ")</f>
         <v xml:space="preserve">INSERT INTO account_holders (user_id, birth_date, main_address_address_id, secondary_address_address_id) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') , '1982-12-02', (SELECT address_id FROM addresses WHERE street LIKE 'Paseo de Montejo' AND house_number LIKE '33') , null); </v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U13" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2581,7 +2583,7 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2592,36 +2594,36 @@
         <v>liliana@email.com</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Liliana') </v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J14" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B14,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Liliana', 'liliana', 'liliana@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2632,36 +2634,36 @@
         <v>maria@email.com</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Maria') </v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J15" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B15,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Maria', 'maria', 'maria@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2672,36 +2674,36 @@
         <v>nancy@email.com</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Nancy') </v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B16,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Nancy', 'nancy', 'nancy@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2712,36 +2714,36 @@
         <v>orlando@email.com</v>
       </c>
       <c r="E17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Orlando') </v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B17,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Orlando', 'orlando', 'orlando@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2752,36 +2754,36 @@
         <v>pedro@email.com</v>
       </c>
       <c r="E18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Pedro') </v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J18" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B18,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Pedro', 'pedro', 'pedro@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2792,36 +2794,36 @@
         <v>quentin@email.com</v>
       </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Quentin') </v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J19" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B19,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Quentin', 'quentin', 'quentin@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2832,39 +2834,39 @@
         <v>ramon@email.com</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ramon') </v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B20,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ramon', 'ramon', 'ramon@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2875,34 +2877,34 @@
         <v>samuel@email.com</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F21" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J21" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B21,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Samuel', 'samuel', 'samuel@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L21" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') , 'ssss'); </v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O21" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2911,7 +2913,7 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2922,34 +2924,34 @@
         <v>tomas@email.com</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F22" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J22" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B22,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Tomas', 'tomas', 'tomas@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L22" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') , 'tttt'); </v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O22" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -2958,7 +2960,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -2969,34 +2971,34 @@
         <v>ubaldo@email.com</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F23" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J23" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B23,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Ubaldo', 'ubaldo', 'ubaldo@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L23" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') , 'uuuu'); </v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O23" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3005,7 +3007,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -3016,34 +3018,34 @@
         <v>veronica@email.com</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F24" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J24" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B24,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Veronica', 'veronica', 'veronica@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L24" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') , 'vvvv'); </v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O24" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3052,7 +3054,7 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -3063,34 +3065,34 @@
         <v>wendy@email.com</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F25" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J25" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B25,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Wendy', 'wendy', 'wendy@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L25" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') , 'wwww'); </v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O25" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3099,7 +3101,7 @@
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -3110,34 +3112,34 @@
         <v>xochil@email.com</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F26" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J26" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B26,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Xochil', 'xochil', 'xochil@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L26" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') , 'xxxx'); </v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O26" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3146,7 +3148,7 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -3157,34 +3159,34 @@
         <v>yolanda@email.com</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F27" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J27" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B27,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Yolanda', 'yolanda', 'yolanda@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L27" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') , 'yyyy'); </v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O27" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3193,7 +3195,7 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="26" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
@@ -3204,34 +3206,34 @@
         <v>zoe@email.com</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F28" s="26" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J28" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",B28,"', '",Tabla4[[#This Row],[username]],"', '",Tabla4[[#This Row],[email]],"', '",Tabla4[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Zoe', 'zoe', 'zoe@email.com', '$2a$10$5VmIyfjdIhdb6GKfIkxwSelOCbI516ZxAfOJic21gHk.KnWE8N.gK'); </v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L28" s="2" t="str">
         <f>CONCATENATE("INSERT INTO third_parties (user_id, hashed_key) VALUES (",Tabla4[[#This Row],[user_id]],", '",Tabla4[[#This Row],[hashed_key]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO third_parties (user_id, hashed_key) VALUES ((SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') , 'zzzz'); </v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O28" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES( (SELECT user_id FROM users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"'), ","( SELECT role_id FROM roles WHERE role_name LIKE '",Tabla4[[#This Row],[Role]],"') ); ")</f>
@@ -3240,22 +3242,22 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3294,50 +3296,50 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="E3" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H3" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="24" t="s">
-        <v>204</v>
-      </c>
       <c r="J3" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3350,23 +3352,23 @@
         <v>23</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H4" s="32">
         <f t="shared" ref="H4:H15" ca="1" si="0">INT(RAND()*1000)</f>
-        <v>335</v>
+        <v>170</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users  WHERE username LIKE '",F4,"') ")</f>
@@ -3377,14 +3379,14 @@
         <v xml:space="preserve">(SELECT user_id FROM users  WHERE username LIKE 'ivan') </v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N4" t="str">
         <f ca="1">CONCATENATE("INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ("," (SELECT user_id FROM users WHERE username LIKE '",E4,"'), ",L4,", '",J4,"', '",G4,"', ",H4,", '",I4,", '",G4,"', ",40," );")</f>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'ivan') , 'CH020', 'EUR', 335, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'ivan') , 'CH020', 'EUR', 170, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -3397,23 +3399,23 @@
         <v>50</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>912</v>
+        <v>286</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K14" si="1">CONCATENATE("(SELECT user_id FROM users  WHERE username LIKE '",F5,"') ")</f>
@@ -3424,14 +3426,14 @@
         <v xml:space="preserve">(SELECT user_id FROM users  WHERE username LIKE 'daniel') </v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N14" ca="1" si="3">CONCATENATE("INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ("," (SELECT user_id FROM users WHERE username LIKE '",E5,"'), ",L5,", '",J5,"', '",G5,"', ",H5,", '",I5,", '",G5,"', ",40," );")</f>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'SA040', 'EUR', 912, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'SA040', 'EUR', 286, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -3444,23 +3446,23 @@
         <v>12</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H6" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>335</v>
+        <v>248</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
@@ -3471,14 +3473,14 @@
         <v xml:space="preserve">(SELECT user_id FROM users  WHERE username LIKE 'daniel') </v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'ST060', 'EUR', 335, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'ST060', 'EUR', 248, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -3491,23 +3493,23 @@
         <v>54</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H7" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>870</v>
+        <v>460</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
@@ -3518,14 +3520,14 @@
         <v xml:space="preserve">(SELECT user_id FROM users  WHERE username LIKE 'hernan') </v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'hernan') , 'CD080', 'EUR', 870, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'hernan') , 'CD080', 'EUR', 460, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -3538,21 +3540,21 @@
         <v>26</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H8" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>346</v>
+        <v>831</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
@@ -3563,14 +3565,14 @@
         <v>null</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH021', 'EUR', 346, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH021', 'EUR', 831, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -3583,21 +3585,21 @@
         <v>11</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H9" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>247</v>
+        <v>894</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
@@ -3608,14 +3610,14 @@
         <v>null</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH022', 'EUR', 247, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH022', 'EUR', 894, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -3628,21 +3630,21 @@
         <v>69</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H10" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>761</v>
+        <v>967</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
@@ -3653,14 +3655,14 @@
         <v>null</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'SA041', 'EUR', 761, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'SA041', 'EUR', 967, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -3673,23 +3675,23 @@
         <v>89</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H11" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>347</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
@@ -3700,14 +3702,14 @@
         <v xml:space="preserve">(SELECT user_id FROM users  WHERE username LIKE 'ernesto') </v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), (SELECT user_id FROM users  WHERE username LIKE 'ernesto') , 'CD081', 'EUR', 347, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), (SELECT user_id FROM users  WHERE username LIKE 'ernesto') , 'CD081', 'EUR', 40, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -3720,21 +3722,21 @@
         <v>24</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H12" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>743</v>
+        <v>54</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
@@ -3745,14 +3747,14 @@
         <v>null</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), null, 'SA042', 'EUR', 743, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), null, 'SA042', 'EUR', 54, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -3765,21 +3767,21 @@
         <v>48</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H13" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>965</v>
+        <v>846</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
@@ -3790,14 +3792,14 @@
         <v>null</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'SA043', 'EUR', 965, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'SA043', 'EUR', 846, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -3810,21 +3812,21 @@
         <v>33</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H14" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>814</v>
+        <v>63</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
@@ -3835,14 +3837,14 @@
         <v>null</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'CH023', 'EUR', 814, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'CH023', 'EUR', 63, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -3851,14 +3853,14 @@
         <v>liliana</v>
       </c>
       <c r="G15" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H15" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>451</v>
+        <v>608</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -3867,14 +3869,14 @@
         <v>maria</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H16" s="32">
         <f t="shared" ref="H16:H29" ca="1" si="4">INT(RAND()*1000)</f>
-        <v>824</v>
+        <v>450</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -3883,14 +3885,14 @@
         <v>nancy</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H17" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>46</v>
+        <v>396</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -3899,52 +3901,52 @@
         <v>orlando</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H18" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>969</v>
+        <v>824</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E19" t="str">
         <f>Users!C18</f>
         <v>pedro</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H19" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>527</v>
+        <v>964</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E20" t="str">
         <f>Users!C19</f>
         <v>quentin</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H20" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>672</v>
+        <v>897</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -3953,14 +3955,14 @@
         <v>ramon</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H21" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>975</v>
+        <v>486</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -3970,19 +3972,19 @@
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H22" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>197</v>
+        <v>469</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E23" s="28" t="str">
         <f>Users!C22</f>
@@ -3990,19 +3992,19 @@
       </c>
       <c r="F23" s="28"/>
       <c r="G23" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H23" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>196</v>
+        <v>487</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E24" s="28" t="str">
         <f>Users!C23</f>
@@ -4010,14 +4012,14 @@
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H24" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>681</v>
+        <v>998</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M24" s="31"/>
     </row>
@@ -4028,14 +4030,14 @@
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H25" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>743</v>
+        <v>71</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -4045,14 +4047,14 @@
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H26" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>989</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -4062,14 +4064,14 @@
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H27" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>907</v>
+        <v>777</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -4079,19 +4081,19 @@
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H28" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>541</v>
+        <v>608</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E29" s="28" t="str">
         <f>Users!C28</f>
@@ -4099,29 +4101,29 @@
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H29" s="32">
         <f t="shared" ca="1" si="4"/>
-        <v>512</v>
+        <v>137</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4154,12 +4156,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J1" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
@@ -4167,7 +4169,7 @@
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="J2" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4175,318 +4177,318 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3">
         <v>23</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3">
         <v>50</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3">
         <v>12</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3">
         <v>54</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3">
         <v>26</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3">
         <v>11</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="3">
         <v>69</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
       </c>
       <c r="E11" s="3">
         <v>89</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I11" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
       </c>
       <c r="E12" s="3">
         <v>24</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
       </c>
       <c r="E13" s="3">
         <v>48</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
       </c>
       <c r="E14" s="3">
         <v>33</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" t="s">
         <v>67</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
       </c>
       <c r="I14" s="11" t="str">
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J15" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J17" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -4494,27 +4496,27 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
         <v>186</v>
       </c>
-      <c r="D19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E19" t="s">
-        <v>188</v>
-      </c>
       <c r="F19" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" s="17" t="s">
         <v>191</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" t="str">
         <f>LOWER(Tabla3[[#This Row],[name]])</f>
@@ -4525,34 +4527,34 @@
         <v>john@email.com</v>
       </c>
       <c r="E20" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I20" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'John') </v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M20" t="str">
         <f>CONCATENATE("INSERT INTO admins VALUES (",K20,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O20" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K20," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
@@ -4561,7 +4563,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="str">
         <f>LOWER(Tabla3[[#This Row],[name]])</f>
@@ -4572,34 +4574,34 @@
         <v>alfredo@email.com</v>
       </c>
       <c r="E21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I21" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K21" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') </v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ref="M21:M23" si="0">CONCATENATE("INSERT INTO admins VALUES (",K21,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
       </c>
       <c r="N21" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O21" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K21," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
@@ -4608,7 +4610,7 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" t="str">
         <f>LOWER(Tabla3[[#This Row],[name]])</f>
@@ -4619,34 +4621,34 @@
         <v>cristian@email.com</v>
       </c>
       <c r="E22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="H22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I22" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K22" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Cristian') </v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
       </c>
       <c r="N22" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O22" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K22," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
@@ -4655,7 +4657,7 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" t="str">
         <f>LOWER(Tabla3[[#This Row],[name]])</f>
@@ -4666,34 +4668,34 @@
         <v>raúl@email.com</v>
       </c>
       <c r="E23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I23" s="11" t="str">
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K23" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users WHERE NAME LIKE '",Tabla3[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM users WHERE NAME LIKE 'Raúl') </v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
       </c>
       <c r="N23" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O23" t="str">
         <f>CONCATENATE("INSERT INTO users_roles (user_id, role_id) VALUES(","( ",K23," ), ( ","SELECT role_id FROM roles WHERE role_name LIKE '",Tabla3[[#This Row],[Rol]],"' ) ); ")</f>
@@ -4702,27 +4704,27 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J24" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J25" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J26" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J27" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J28" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 'External Resources':  - Added png image for 'uses cases' diagram.  - Added png image for 'Class diagram' of the entire project.  - Updated 'Requirements and Instructions.docx' reflecting the accomplished objectives of the requirements.  - 'Mapa Endpoints.xlsx' updated showing the new endpoints and their URL to access each of those.    #1
</commit_message>
<xml_diff>
--- a/External_Resources/Mapa Endpoints.xlsx
+++ b/External_Resources/Mapa Endpoints.xlsx
@@ -509,15 +509,6 @@
     <t>IBAN, anterior saldo, nuevo saldo</t>
   </si>
   <si>
-    <t>/accountholder/{id}/{IBAN}</t>
-  </si>
-  <si>
-    <t>/accountholder/{id}/{IBAN}?transaction={X}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar transferencia </t>
-  </si>
-  <si>
     <t>ThirdParty</t>
   </si>
   <si>
@@ -744,6 +735,15 @@
   </si>
   <si>
     <t>Muestra las cuentas del usuario</t>
+  </si>
+  <si>
+    <t>/accountholder/{IBAN}</t>
+  </si>
+  <si>
+    <t>/accountholder/{IBAN}/transfer</t>
+  </si>
+  <si>
+    <t>Realizar transferencia entre dos cuentas.</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -935,7 +935,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1392,7 +1391,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,13 +1406,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1445,8 +1444,8 @@
       <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>197</v>
+      <c r="E4" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
@@ -1459,14 +1458,14 @@
       <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>174</v>
+      <c r="E5" s="13" t="s">
+        <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,14 +1478,14 @@
       <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>173</v>
+      <c r="E6" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="F6" t="s">
         <v>142</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,10 +1533,10 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>143</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1554,11 +1553,11 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>169</v>
+      <c r="E13" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
@@ -1574,10 +1573,10 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>144</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1591,10 +1590,10 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>145</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1605,11 +1604,11 @@
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>170</v>
+      <c r="E16" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>19</v>
@@ -1622,11 +1621,11 @@
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>211</v>
+      <c r="E17" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>18</v>
@@ -1636,11 +1635,11 @@
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>170</v>
+      <c r="E18" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>22</v>
@@ -1653,48 +1652,48 @@
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" t="s">
         <v>179</v>
-      </c>
-      <c r="G19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" t="s">
         <v>180</v>
-      </c>
-      <c r="G20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1713,25 +1712,25 @@
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>237</v>
+      <c r="E24" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>160</v>
+        <v>236</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>18</v>
@@ -1741,17 +1740,17 @@
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>161</v>
+      <c r="E26" s="13" t="s">
+        <v>237</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>162</v>
+        <v>238</v>
       </c>
       <c r="G26" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1761,19 +1760,19 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" t="s">
         <v>163</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G28" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1833,13 +1832,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F2" t="s">
         <v>74</v>
@@ -1848,7 +1847,7 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>25</v>
@@ -1859,39 +1858,39 @@
       <c r="O2" t="s">
         <v>139</v>
       </c>
-      <c r="S2" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>195</v>
+      <c r="S2" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="U2" s="20" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="17" t="str">
+      <c r="C3" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>alberto</v>
       </c>
-      <c r="D3" s="17" t="str">
+      <c r="D3" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>alberto@email.com</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F3" s="17" t="str">
+      <c r="E3" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Alberto') </v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J3" s="11" t="str">
@@ -1932,31 +1931,31 @@
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="17" t="str">
+      <c r="C4" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>bernardo</v>
       </c>
-      <c r="D4" s="17" t="str">
+      <c r="D4" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>bernardo@email.com</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F4" s="17" t="str">
+      <c r="E4" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Bernardo') </v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="19" t="s">
+      <c r="H4" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J4" s="11" t="str">
@@ -1997,31 +1996,31 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="17" t="str">
+      <c r="C5" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>carlos</v>
       </c>
-      <c r="D5" s="17" t="str">
+      <c r="D5" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>carlos@email.com</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="17" t="str">
+      <c r="E5" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Carlos') </v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J5" s="11" t="str">
@@ -2062,31 +2061,31 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="17" t="str">
+      <c r="C6" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>daniel</v>
       </c>
-      <c r="D6" s="17" t="str">
+      <c r="D6" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>daniel@email.com</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="17" t="str">
+      <c r="E6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Daniel') </v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="H6" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J6" s="11" t="str">
@@ -2127,31 +2126,31 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="17" t="str">
+      <c r="C7" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>ernesto</v>
       </c>
-      <c r="D7" s="17" t="str">
+      <c r="D7" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ernesto@email.com</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F7" s="17" t="str">
+      <c r="E7" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ernesto') </v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J7" s="11" t="str">
@@ -2192,31 +2191,31 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="17" t="str">
+      <c r="C8" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>fernando</v>
       </c>
-      <c r="D8" s="17" t="str">
+      <c r="D8" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>fernando@email.com</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F8" s="17" t="str">
+      <c r="E8" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Fernando') </v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J8" s="11" t="str">
@@ -2257,31 +2256,31 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="17" t="str">
+      <c r="C9" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>gladys</v>
       </c>
-      <c r="D9" s="17" t="str">
+      <c r="D9" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>gladys@email.com</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="17" t="str">
+      <c r="E9" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Gladys') </v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J9" s="11" t="str">
@@ -2322,31 +2321,31 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="17" t="str">
+      <c r="C10" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>hernan</v>
       </c>
-      <c r="D10" s="17" t="str">
+      <c r="D10" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>hernan@email.com</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F10" s="17" t="str">
+      <c r="E10" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Hernan') </v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I10" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J10" s="11" t="str">
@@ -2387,31 +2386,31 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="17" t="str">
+      <c r="C11" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>ivan</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ivan@email.com</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F11" s="17" t="str">
+      <c r="E11" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F11" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ivan') </v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I11" s="19" t="s">
+      <c r="H11" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I11" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J11" s="11" t="str">
@@ -2452,31 +2451,31 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>jose</v>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>jose@email.com</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F12" s="17" t="str">
+      <c r="E12" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Jose') </v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J12" s="11" t="str">
@@ -2517,31 +2516,31 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="17" t="str">
+      <c r="C13" s="16" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>kevin</v>
       </c>
-      <c r="D13" s="17" t="str">
+      <c r="D13" s="16" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>kevin@email.com</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="17" t="str">
+      <c r="E13" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Kevin') </v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J13" s="11" t="str">
@@ -2594,7 +2593,7 @@
         <v>liliana@email.com</v>
       </c>
       <c r="E14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F14" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2603,8 +2602,8 @@
       <c r="G14" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J14" s="11" t="str">
@@ -2634,7 +2633,7 @@
         <v>maria@email.com</v>
       </c>
       <c r="E15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F15" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2643,8 +2642,8 @@
       <c r="G15" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19" t="s">
+      <c r="H15" s="17"/>
+      <c r="I15" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J15" s="11" t="str">
@@ -2674,7 +2673,7 @@
         <v>nancy@email.com</v>
       </c>
       <c r="E16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F16" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2683,8 +2682,8 @@
       <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="19" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J16" s="11" t="str">
@@ -2714,7 +2713,7 @@
         <v>orlando@email.com</v>
       </c>
       <c r="E17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F17" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2723,8 +2722,8 @@
       <c r="G17" t="s">
         <v>115</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="17"/>
+      <c r="I17" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J17" s="11" t="str">
@@ -2754,7 +2753,7 @@
         <v>pedro@email.com</v>
       </c>
       <c r="E18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F18" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2763,8 +2762,8 @@
       <c r="G18" t="s">
         <v>116</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19" t="s">
+      <c r="H18" s="17"/>
+      <c r="I18" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J18" s="11" t="str">
@@ -2794,7 +2793,7 @@
         <v>quentin@email.com</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F19" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2803,8 +2802,8 @@
       <c r="G19" t="s">
         <v>117</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="17"/>
+      <c r="I19" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J19" s="11" t="str">
@@ -2834,7 +2833,7 @@
         <v>ramon@email.com</v>
       </c>
       <c r="E20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F20" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
@@ -2843,8 +2842,8 @@
       <c r="G20" t="s">
         <v>118</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="19" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J20" s="11" t="str">
@@ -2854,8 +2853,8 @@
       <c r="K20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="O20" s="21" t="s">
-        <v>195</v>
+      <c r="O20" s="20" t="s">
+        <v>192</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>140</v>
@@ -2865,31 +2864,31 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="26" t="str">
+      <c r="C21" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>samuel</v>
       </c>
-      <c r="D21" s="26" t="str">
+      <c r="D21" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>samuel@email.com</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F21" s="26" t="str">
+      <c r="E21" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Samuel') </v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J21" s="11" t="str">
@@ -2912,31 +2911,31 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="26" t="str">
+      <c r="C22" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>tomas</v>
       </c>
-      <c r="D22" s="26" t="str">
+      <c r="D22" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>tomas@email.com</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F22" s="26" t="str">
+      <c r="E22" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Tomas') </v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H22" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I22" s="19" t="s">
+      <c r="H22" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J22" s="11" t="str">
@@ -2959,31 +2958,31 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="26" t="str">
+      <c r="C23" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>ubaldo</v>
       </c>
-      <c r="D23" s="26" t="str">
+      <c r="D23" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>ubaldo@email.com</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F23" s="26" t="str">
+      <c r="E23" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Ubaldo') </v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I23" s="19" t="s">
+      <c r="H23" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J23" s="11" t="str">
@@ -3006,31 +3005,31 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="26" t="str">
+      <c r="C24" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>veronica</v>
       </c>
-      <c r="D24" s="26" t="str">
+      <c r="D24" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>veronica@email.com</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F24" s="26" t="str">
+      <c r="E24" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Veronica') </v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I24" s="19" t="s">
+      <c r="H24" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J24" s="11" t="str">
@@ -3053,31 +3052,31 @@
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="26" t="str">
+      <c r="C25" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>wendy</v>
       </c>
-      <c r="D25" s="26" t="str">
+      <c r="D25" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>wendy@email.com</v>
       </c>
-      <c r="E25" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F25" s="26" t="str">
+      <c r="E25" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Wendy') </v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="H25" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I25" s="19" t="s">
+      <c r="H25" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J25" s="11" t="str">
@@ -3100,31 +3099,31 @@
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="26" t="str">
+      <c r="C26" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>xochil</v>
       </c>
-      <c r="D26" s="26" t="str">
+      <c r="D26" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>xochil@email.com</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F26" s="26" t="str">
+      <c r="E26" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F26" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Xochil') </v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="H26" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I26" s="19" t="s">
+      <c r="H26" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J26" s="11" t="str">
@@ -3147,31 +3146,31 @@
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="26" t="str">
+      <c r="C27" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>yolanda</v>
       </c>
-      <c r="D27" s="26" t="str">
+      <c r="D27" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>yolanda@email.com</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F27" s="26" t="str">
+      <c r="E27" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F27" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Yolanda') </v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I27" s="19" t="s">
+      <c r="H27" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J27" s="11" t="str">
@@ -3194,31 +3193,31 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="26" t="str">
+      <c r="C28" s="25" t="str">
         <f>LOWER(Tabla4[[#This Row],[name]])</f>
         <v>zoe</v>
       </c>
-      <c r="D28" s="26" t="str">
+      <c r="D28" s="25" t="str">
         <f>CONCATENATE(Tabla4[[#This Row],[username]],"@email.com")</f>
         <v>zoe@email.com</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="F28" s="26" t="str">
+      <c r="E28" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="25" t="str">
         <f>CONCATENATE("(SELECT user_id FROM  users WHERE NAME LIKE '",Tabla4[[#This Row],[name]],"') ")</f>
         <v xml:space="preserve">(SELECT user_id FROM  users WHERE NAME LIKE 'Zoe') </v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I28" s="19" t="s">
+      <c r="H28" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I28" s="18" t="s">
         <v>140</v>
       </c>
       <c r="J28" s="11" t="str">
@@ -3242,22 +3241,22 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3275,7 +3274,7 @@
   <dimension ref="B1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,7 +3282,7 @@
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="29" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
@@ -3296,12 +3295,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3311,35 +3310,35 @@
       <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="E3" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="J3" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="I3" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="L3" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>236</v>
+      <c r="N3" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3351,24 +3350,24 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>23</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H4" s="32">
+      <c r="E4" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="31">
         <f t="shared" ref="H4:H15" ca="1" si="0">INT(RAND()*1000)</f>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE("(SELECT user_id FROM users  WHERE username LIKE '",F4,"') ")</f>
@@ -3383,7 +3382,7 @@
       </c>
       <c r="N4" t="str">
         <f ca="1">CONCATENATE("INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ("," (SELECT user_id FROM users WHERE username LIKE '",E4,"'), ",L4,", '",J4,"', '",G4,"', ",H4,", '",I4,", '",G4,"', ",40," );")</f>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'ivan') , 'CH020', 'EUR', 170, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'ivan') , 'CH020', 'EUR', 180, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>140</v>
@@ -3398,24 +3397,24 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>50</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H5" s="32">
+      <c r="E5" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>286</v>
+        <v>181</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K14" si="1">CONCATENATE("(SELECT user_id FROM users  WHERE username LIKE '",F5,"') ")</f>
@@ -3430,7 +3429,7 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N14" ca="1" si="3">CONCATENATE("INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ("," (SELECT user_id FROM users WHERE username LIKE '",E5,"'), ",L5,", '",J5,"', '",G5,"', ",H5,", '",I5,", '",G5,"', ",40," );")</f>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'SA040', 'EUR', 286, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'SA040', 'EUR', 181, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>140</v>
@@ -3445,24 +3444,24 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>12</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H6" s="32">
+      <c r="E6" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>248</v>
+        <v>66</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
@@ -3477,7 +3476,7 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'ST060', 'EUR', 248, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'daniel') , 'ST060', 'EUR', 66, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>140</v>
@@ -3492,24 +3491,24 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>54</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H7" s="32">
+      <c r="E7" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H7" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>460</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
@@ -3524,7 +3523,7 @@
       </c>
       <c r="N7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'hernan') , 'CD080', 'EUR', 460, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'alberto'), (SELECT user_id FROM users  WHERE username LIKE 'hernan') , 'CD080', 'EUR', 1, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>140</v>
@@ -3539,22 +3538,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>26</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H8" s="32">
+      <c r="E8" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>831</v>
+        <v>443</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
@@ -3569,7 +3568,7 @@
       </c>
       <c r="N8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH021', 'EUR', 831, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH021', 'EUR', 443, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>140</v>
@@ -3584,22 +3583,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>11</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H9" s="32">
+      <c r="E9" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>894</v>
+        <v>680</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
@@ -3614,7 +3613,7 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH022', 'EUR', 894, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'CH022', 'EUR', 680, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>140</v>
@@ -3629,22 +3628,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>69</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H10" s="32">
+      <c r="E10" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>967</v>
+        <v>671</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
@@ -3659,7 +3658,7 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'SA041', 'EUR', 967, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ernesto'), null, 'SA041', 'EUR', 671, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>140</v>
@@ -3674,24 +3673,24 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>89</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H11" s="32">
+      <c r="E11" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
@@ -3706,7 +3705,7 @@
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), (SELECT user_id FROM users  WHERE username LIKE 'ernesto') , 'CD081', 'EUR', 40, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), (SELECT user_id FROM users  WHERE username LIKE 'ernesto') , 'CD081', 'EUR', 158, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>140</v>
@@ -3721,22 +3720,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>24</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H12" s="32">
+      <c r="E12" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>174</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
@@ -3751,7 +3750,7 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), null, 'SA042', 'EUR', 54, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'ivan'), null, 'SA042', 'EUR', 174, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>140</v>
@@ -3766,22 +3765,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>48</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H13" s="32">
+      <c r="E13" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>846</v>
+        <v>646</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
@@ -3796,7 +3795,7 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'SA043', 'EUR', 846, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'SA043', 'EUR', 646, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>140</v>
@@ -3811,22 +3810,22 @@
         <f>Tabla1[[#This Row],[house_number]]</f>
         <v>33</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H14" s="32">
+      <c r="E14" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
@@ -3841,7 +3840,7 @@
       </c>
       <c r="N14" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'CH023', 'EUR', 63, '2022-11-01 20:07:29', 'EUR', 40 );</v>
+        <v>INSERT INTO basic_accounts (first_account_holder_user_id, second_accountholder_user_id, iban, currency, amount, creation_time, currency_penalty_fee, amount_penalty_fee) VALUES ( (SELECT user_id FROM users WHERE username LIKE 'kevin'), null, 'CH023', 'EUR', 148, '2022-11-01 20:07:29', 'EUR', 40 );</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>140</v>
@@ -3852,15 +3851,15 @@
         <f>Users!C14</f>
         <v>liliana</v>
       </c>
-      <c r="G15" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H15" s="32">
+      <c r="G15" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>608</v>
+        <v>454</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -3868,15 +3867,15 @@
         <f>Users!C15</f>
         <v>maria</v>
       </c>
-      <c r="G16" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H16" s="32">
+      <c r="G16" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="31">
         <f t="shared" ref="H16:H29" ca="1" si="4">INT(RAND()*1000)</f>
-        <v>450</v>
+        <v>153</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -3884,15 +3883,15 @@
         <f>Users!C16</f>
         <v>nancy</v>
       </c>
-      <c r="G17" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H17" s="32">
+      <c r="G17" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>396</v>
+        <v>446</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -3900,53 +3899,53 @@
         <f>Users!C17</f>
         <v>orlando</v>
       </c>
-      <c r="G18" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H18" s="32">
+      <c r="G18" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H18" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>824</v>
+        <v>73</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E19" t="str">
         <f>Users!C18</f>
         <v>pedro</v>
       </c>
-      <c r="G19" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H19" s="32">
+      <c r="G19" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H19" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>964</v>
+        <v>214</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E20" t="str">
         <f>Users!C19</f>
         <v>quentin</v>
       </c>
-      <c r="G20" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H20" s="32">
+      <c r="G20" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H20" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>897</v>
+        <v>484</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -3954,176 +3953,176 @@
         <f>Users!C20</f>
         <v>ramon</v>
       </c>
-      <c r="G21" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H21" s="32">
+      <c r="G21" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H21" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>567</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E22" s="28" t="str">
+      <c r="E22" s="27" t="str">
         <f>Users!C21</f>
         <v>samuel</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H22" s="32">
+      <c r="F22" s="27"/>
+      <c r="G22" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>469</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>206</v>
-      </c>
-      <c r="E23" s="28" t="str">
+        <v>203</v>
+      </c>
+      <c r="E23" s="27" t="str">
         <f>Users!C22</f>
         <v>tomas</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H23" s="32">
+      <c r="F23" s="27"/>
+      <c r="G23" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H23" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>487</v>
+        <v>927</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>207</v>
-      </c>
-      <c r="E24" s="28" t="str">
+        <v>204</v>
+      </c>
+      <c r="E24" s="27" t="str">
         <f>Users!C23</f>
         <v>ubaldo</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H24" s="32">
+      <c r="F24" s="27"/>
+      <c r="G24" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H24" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>998</v>
+        <v>950</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="M24" s="31"/>
+        <v>207</v>
+      </c>
+      <c r="M24" s="30"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E25" s="28" t="str">
+      <c r="E25" s="27" t="str">
         <f>Users!C24</f>
         <v>veronica</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H25" s="32">
+      <c r="F25" s="27"/>
+      <c r="G25" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>227</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E26" s="28" t="str">
+      <c r="E26" s="27" t="str">
         <f>Users!C25</f>
         <v>wendy</v>
       </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H26" s="32">
+      <c r="F26" s="27"/>
+      <c r="G26" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H26" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>989</v>
+        <v>238</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E27" s="28" t="str">
+      <c r="E27" s="27" t="str">
         <f>Users!C26</f>
         <v>xochil</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H27" s="32">
+      <c r="F27" s="27"/>
+      <c r="G27" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H27" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>777</v>
+        <v>978</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E28" s="28" t="str">
+      <c r="E28" s="27" t="str">
         <f>Users!C27</f>
         <v>yolanda</v>
       </c>
-      <c r="F28" s="28"/>
-      <c r="G28" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H28" s="32">
+      <c r="F28" s="27"/>
+      <c r="G28" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>608</v>
+        <v>691</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="28" t="str">
+        <v>209</v>
+      </c>
+      <c r="E29" s="27" t="str">
         <f>Users!C28</f>
         <v>zoe</v>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="H29" s="32">
+      <c r="F29" s="27"/>
+      <c r="G29" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>137</v>
+        <v>362</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4155,20 +4154,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="J2" s="16" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="J2" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4194,10 +4193,10 @@
       <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J3" s="16" t="s">
+      <c r="I3" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4221,7 +4220,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Numancia', '23', '4-2', '' ); </v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4245,7 +4244,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Madrid', 'Gran Via', '50', '3-1', '' ); </v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4269,7 +4268,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Barcelona', 'Napoles', '12', 'Bajos 3', '' ); </v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4293,7 +4292,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Valencia', 'Dénia', '54', 'Atico', '' ); </v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4317,7 +4316,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('España', 'Badajoz', 'San Blas', '26', '2-1', '' ); </v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4341,7 +4340,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Francia', 'Paris', 'Rivolí', '11', '3-3', '' ); </v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4365,7 +4364,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Alemania', 'Frankfurt', 'Oberweg', '69', '3 ', '' ); </v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4389,7 +4388,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Colombia', 'Bogotá', 'Av El Dorado', '89', 'apto 3', '' ); </v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4413,7 +4412,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Peru', 'Lima', 'Jirón Callao', '24', 'A ', '' ); </v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4437,7 +4436,7 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Argentina', 'Buenos Aires', 'Av 9 de Julio', '48', 'Apto 2', '' ); </v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4464,22 +4463,22 @@
         <f>CONCATENATE("INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('",Tabla1[[#This Row],[country]],"', '",Tabla1[[#This Row],[city]],"', '",Tabla1[[#This Row],[street]],"', '",Tabla1[[#This Row],[house_number]],"', '",Tabla1[[#This Row],[home_unit]],"', '",Tabla1[[#This Row],[comment]],"' ); ")</f>
         <v xml:space="preserve">INSERT INTO addresses (country, city, street, house_number, home_unit, COMMENT)   VALUES ('Mexico', 'Merida', 'Paseo de Montejo', '33', 'Casa Azul', 'Al lado del monumento' ); </v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4487,7 +4486,7 @@
       <c r="B18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4496,22 +4495,22 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>191</v>
+      <c r="J19" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -4527,10 +4526,10 @@
         <v>john@email.com</v>
       </c>
       <c r="E20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>140</v>
@@ -4539,7 +4538,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('John', 'john', 'john@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="15" t="s">
         <v>140</v>
       </c>
       <c r="K20" t="str">
@@ -4553,7 +4552,7 @@
         <f>CONCATENATE("INSERT INTO admins VALUES (",K20,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'John') ); </v>
       </c>
-      <c r="N20" s="16" t="s">
+      <c r="N20" s="15" t="s">
         <v>140</v>
       </c>
       <c r="O20" t="str">
@@ -4574,10 +4573,10 @@
         <v>alfredo@email.com</v>
       </c>
       <c r="E21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>140</v>
@@ -4586,7 +4585,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Alfredo', 'alfredo', 'alfredo@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="15" t="s">
         <v>140</v>
       </c>
       <c r="K21" t="str">
@@ -4600,7 +4599,7 @@
         <f t="shared" ref="M21:M23" si="0">CONCATENATE("INSERT INTO admins VALUES (",K21,"); ")</f>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Alfredo') ); </v>
       </c>
-      <c r="N21" s="16" t="s">
+      <c r="N21" s="15" t="s">
         <v>140</v>
       </c>
       <c r="O21" t="str">
@@ -4621,10 +4620,10 @@
         <v>cristian@email.com</v>
       </c>
       <c r="E22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>140</v>
@@ -4633,7 +4632,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Cristian', 'cristian', 'cristian@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="J22" s="15" t="s">
         <v>140</v>
       </c>
       <c r="K22" t="str">
@@ -4647,7 +4646,7 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Cristian') ); </v>
       </c>
-      <c r="N22" s="16" t="s">
+      <c r="N22" s="15" t="s">
         <v>140</v>
       </c>
       <c r="O22" t="str">
@@ -4668,10 +4667,10 @@
         <v>raúl@email.com</v>
       </c>
       <c r="E23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>140</v>
@@ -4680,7 +4679,7 @@
         <f>CONCATENATE("INSERT INTO users (name, username, email, password) VALUES ('",Tabla3[[#This Row],[name]],"', '",Tabla3[[#This Row],[username]],"', '",Tabla3[[#This Row],[email]],"', '",Tabla3[[#This Row],[password]],"'); ")</f>
         <v xml:space="preserve">INSERT INTO users (name, username, email, password) VALUES ('Raúl', 'raúl', 'raúl@email.com', '$2a$10$EmDCvndz9V.qV4s48TCXYOplNJc54si3hM2yby.stIO3ETgMoWFbS'); </v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="15" t="s">
         <v>140</v>
       </c>
       <c r="K23" t="str">
@@ -4694,7 +4693,7 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">INSERT INTO admins VALUES ((SELECT user_id FROM users WHERE NAME LIKE 'Raúl') ); </v>
       </c>
-      <c r="N23" s="16" t="s">
+      <c r="N23" s="15" t="s">
         <v>140</v>
       </c>
       <c r="O23" t="str">
@@ -4703,27 +4702,27 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J26" s="16" t="s">
+      <c r="J26" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="16" t="s">
+      <c r="J27" s="15" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J28" s="16" t="s">
+      <c r="J28" s="15" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>